<commit_message>
pembaruan menambahkan data baru dan interpretasi nya
</commit_message>
<xml_diff>
--- a/JST_AGUN_FIRMANSYAH_22112012.xlsx
+++ b/JST_AGUN_FIRMANSYAH_22112012.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Semester_6\JST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9ED6ACD-2696-49FD-B95D-E7900838EC49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11DB4528-67D0-45BA-A6D0-3B015D89C577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{B70DD9B1-ECAE-45D8-BEBA-901DEA88A266}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1313" uniqueCount="171">
   <si>
     <t>McP Tanpa Bias</t>
   </si>
@@ -539,6 +539,96 @@
   </si>
   <si>
     <t>w4 awal</t>
+  </si>
+  <si>
+    <t>data baru</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>Aspek</t>
+  </si>
+  <si>
+    <t>Isi</t>
+  </si>
+  <si>
+    <t>Bobot Awal</t>
+  </si>
+  <si>
+    <t>w1=-0.8, w2=-11, w3=-10, w4=-5</t>
+  </si>
+  <si>
+    <t>Bias Awal</t>
+  </si>
+  <si>
+    <t>bias=-5</t>
+  </si>
+  <si>
+    <t>Jumlah Data Latih</t>
+  </si>
+  <si>
+    <t>Algoritma yang Digunakan</t>
+  </si>
+  <si>
+    <t>Hebb Rule</t>
+  </si>
+  <si>
+    <t>Fungsi Aktivasi</t>
+  </si>
+  <si>
+    <t>Bipolar (1 jika Y_in&gt;0, -1 jika Y_in&lt;=0)</t>
+  </si>
+  <si>
+    <t>Kondisi Aktivasi</t>
+  </si>
+  <si>
+    <t>Y = 1 jika Y_in &gt; 0, Y = -1 jika Y_in &lt;= 0</t>
+  </si>
+  <si>
+    <t>Bobot Akhir</t>
+  </si>
+  <si>
+    <t>w1=8.2, w2=-4.25, w3=-7.25, w4=-2.25</t>
+  </si>
+  <si>
+    <t>Bias Akhir</t>
+  </si>
+  <si>
+    <t>bias=4</t>
+  </si>
+  <si>
+    <t>Hasil Uji (16 Data Latih)</t>
+  </si>
+  <si>
+    <t>Berhasil untuk sebagian besar data, gagal di 1 data</t>
+  </si>
+  <si>
+    <t>Hasil Uji (Data Baru 17)</t>
+  </si>
+  <si>
+    <t>Y_in = 5.95 → Y = 1 ✅</t>
+  </si>
+  <si>
+    <t>Hasil Uji (Data Baru 18)</t>
+  </si>
+  <si>
+    <t>Y_in = -2.7 → Y = 0 ❌</t>
+  </si>
+  <si>
+    <t>Kesimpulan</t>
+  </si>
+  <si>
+    <t>JST Hebb Rule hanya mampu memetakan logika AND untuk 1 kombinasi input saja</t>
+  </si>
+  <si>
+    <t>Catatan Tambahan</t>
+  </si>
+  <si>
+    <t>Hebb Rule sederhana, tidak mampu menangani kesalahan atau logika kompleks seperti XOR</t>
   </si>
 </sst>
 </file>
@@ -1161,10 +1251,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1401,6 +1492,12 @@
     <xf numFmtId="0" fontId="2" fillId="18" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="29" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="29" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1413,6 +1510,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1422,14 +1528,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1438,12 +1544,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1473,18 +1573,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="29" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="29" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{8572C7AC-D6D0-44A3-B2AB-846548AB2057}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1895,7 +1991,7 @@
       <c r="D4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="90" t="s">
+      <c r="E4" s="92" t="s">
         <v>6</v>
       </c>
       <c r="F4" s="2" t="s">
@@ -1929,7 +2025,7 @@
         <v>0.4</v>
       </c>
       <c r="D5" s="2"/>
-      <c r="E5" s="91"/>
+      <c r="E5" s="93"/>
       <c r="F5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2253,7 +2349,7 @@
       <c r="D15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E15" s="90" t="s">
+      <c r="E15" s="92" t="s">
         <v>6</v>
       </c>
       <c r="F15" s="2" t="s">
@@ -2287,7 +2383,7 @@
         <v>2</v>
       </c>
       <c r="D16" s="2"/>
-      <c r="E16" s="91"/>
+      <c r="E16" s="93"/>
       <c r="F16" s="2" t="s">
         <v>9</v>
       </c>
@@ -2611,7 +2707,7 @@
       <c r="D26" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E26" s="90" t="s">
+      <c r="E26" s="92" t="s">
         <v>6</v>
       </c>
       <c r="F26" s="2" t="s">
@@ -2645,7 +2741,7 @@
         <v>-2</v>
       </c>
       <c r="D27" s="2"/>
-      <c r="E27" s="91"/>
+      <c r="E27" s="93"/>
       <c r="F27" s="2" t="s">
         <v>9</v>
       </c>
@@ -2969,7 +3065,7 @@
       <c r="D37" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E37" s="90" t="s">
+      <c r="E37" s="92" t="s">
         <v>6</v>
       </c>
       <c r="F37" s="2" t="s">
@@ -3003,7 +3099,7 @@
         <v>-2</v>
       </c>
       <c r="D38" s="2"/>
-      <c r="E38" s="91"/>
+      <c r="E38" s="93"/>
       <c r="F38" s="2" t="s">
         <v>9</v>
       </c>
@@ -7770,61 +7866,61 @@
       <c r="AG8" s="2"/>
     </row>
     <row r="9" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="92" t="s">
+      <c r="A9" s="94" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="94" t="s">
+      <c r="B9" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="95"/>
-      <c r="D9" s="96"/>
-      <c r="E9" s="92" t="s">
+      <c r="C9" s="100"/>
+      <c r="D9" s="101"/>
+      <c r="E9" s="94" t="s">
         <v>55</v>
       </c>
-      <c r="F9" s="94" t="s">
+      <c r="F9" s="99" t="s">
         <v>56</v>
       </c>
-      <c r="G9" s="95"/>
-      <c r="H9" s="96"/>
-      <c r="I9" s="94" t="s">
+      <c r="G9" s="100"/>
+      <c r="H9" s="101"/>
+      <c r="I9" s="99" t="s">
         <v>57</v>
       </c>
-      <c r="J9" s="95"/>
-      <c r="K9" s="96"/>
-      <c r="L9" s="92" t="s">
+      <c r="J9" s="100"/>
+      <c r="K9" s="101"/>
+      <c r="L9" s="94" t="s">
         <v>58</v>
       </c>
-      <c r="M9" s="92" t="s">
+      <c r="M9" s="94" t="s">
         <v>59</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
-      <c r="R9" s="92" t="s">
+      <c r="R9" s="94" t="s">
         <v>53</v>
       </c>
-      <c r="S9" s="94" t="s">
+      <c r="S9" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="T9" s="95"/>
-      <c r="U9" s="96"/>
-      <c r="V9" s="92" t="s">
+      <c r="T9" s="100"/>
+      <c r="U9" s="101"/>
+      <c r="V9" s="94" t="s">
         <v>55</v>
       </c>
-      <c r="W9" s="94" t="s">
+      <c r="W9" s="99" t="s">
         <v>56</v>
       </c>
-      <c r="X9" s="95"/>
-      <c r="Y9" s="96"/>
-      <c r="Z9" s="94" t="s">
+      <c r="X9" s="100"/>
+      <c r="Y9" s="101"/>
+      <c r="Z9" s="99" t="s">
         <v>57</v>
       </c>
-      <c r="AA9" s="95"/>
-      <c r="AB9" s="96"/>
-      <c r="AC9" s="92" t="s">
+      <c r="AA9" s="100"/>
+      <c r="AB9" s="101"/>
+      <c r="AC9" s="94" t="s">
         <v>58</v>
       </c>
-      <c r="AD9" s="92" t="s">
+      <c r="AD9" s="94" t="s">
         <v>59</v>
       </c>
       <c r="AE9" s="2"/>
@@ -7832,7 +7928,7 @@
       <c r="AG9" s="2"/>
     </row>
     <row r="10" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="93"/>
+      <c r="A10" s="95"/>
       <c r="B10" s="34" t="s">
         <v>13</v>
       </c>
@@ -7842,7 +7938,7 @@
       <c r="D10" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="E10" s="93"/>
+      <c r="E10" s="95"/>
       <c r="F10" s="34" t="s">
         <v>33</v>
       </c>
@@ -7861,12 +7957,12 @@
       <c r="K10" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="L10" s="93"/>
-      <c r="M10" s="93"/>
+      <c r="L10" s="95"/>
+      <c r="M10" s="95"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
-      <c r="R10" s="93"/>
+      <c r="R10" s="95"/>
       <c r="S10" s="34" t="s">
         <v>13</v>
       </c>
@@ -7876,7 +7972,7 @@
       <c r="U10" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="V10" s="93"/>
+      <c r="V10" s="95"/>
       <c r="W10" s="34" t="s">
         <v>33</v>
       </c>
@@ -7895,8 +7991,8 @@
       <c r="AB10" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="AC10" s="93"/>
-      <c r="AD10" s="93"/>
+      <c r="AC10" s="95"/>
+      <c r="AD10" s="95"/>
       <c r="AE10" s="2"/>
       <c r="AF10" s="2"/>
       <c r="AG10" s="2"/>
@@ -8854,61 +8950,61 @@
       <c r="AG28" s="2"/>
     </row>
     <row r="29" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="92" t="s">
+      <c r="A29" s="94" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="94" t="s">
+      <c r="B29" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="C29" s="95"/>
-      <c r="D29" s="96"/>
-      <c r="E29" s="92" t="s">
+      <c r="C29" s="100"/>
+      <c r="D29" s="101"/>
+      <c r="E29" s="94" t="s">
         <v>55</v>
       </c>
-      <c r="F29" s="94" t="s">
+      <c r="F29" s="99" t="s">
         <v>56</v>
       </c>
-      <c r="G29" s="95"/>
-      <c r="H29" s="96"/>
-      <c r="I29" s="94" t="s">
+      <c r="G29" s="100"/>
+      <c r="H29" s="101"/>
+      <c r="I29" s="99" t="s">
         <v>57</v>
       </c>
-      <c r="J29" s="95"/>
-      <c r="K29" s="96"/>
-      <c r="L29" s="92" t="s">
+      <c r="J29" s="100"/>
+      <c r="K29" s="101"/>
+      <c r="L29" s="94" t="s">
         <v>58</v>
       </c>
-      <c r="M29" s="92" t="s">
+      <c r="M29" s="94" t="s">
         <v>59</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
       <c r="P29" s="2"/>
-      <c r="R29" s="92" t="s">
+      <c r="R29" s="94" t="s">
         <v>53</v>
       </c>
-      <c r="S29" s="94" t="s">
+      <c r="S29" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="T29" s="95"/>
-      <c r="U29" s="96"/>
-      <c r="V29" s="92" t="s">
+      <c r="T29" s="100"/>
+      <c r="U29" s="101"/>
+      <c r="V29" s="94" t="s">
         <v>55</v>
       </c>
-      <c r="W29" s="94" t="s">
+      <c r="W29" s="99" t="s">
         <v>56</v>
       </c>
-      <c r="X29" s="95"/>
-      <c r="Y29" s="96"/>
-      <c r="Z29" s="94" t="s">
+      <c r="X29" s="100"/>
+      <c r="Y29" s="101"/>
+      <c r="Z29" s="99" t="s">
         <v>57</v>
       </c>
-      <c r="AA29" s="95"/>
-      <c r="AB29" s="96"/>
-      <c r="AC29" s="92" t="s">
+      <c r="AA29" s="100"/>
+      <c r="AB29" s="101"/>
+      <c r="AC29" s="94" t="s">
         <v>58</v>
       </c>
-      <c r="AD29" s="92" t="s">
+      <c r="AD29" s="94" t="s">
         <v>59</v>
       </c>
       <c r="AE29" s="2"/>
@@ -8916,7 +9012,7 @@
       <c r="AG29" s="2"/>
     </row>
     <row r="30" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="93"/>
+      <c r="A30" s="95"/>
       <c r="B30" s="34" t="s">
         <v>13</v>
       </c>
@@ -8926,7 +9022,7 @@
       <c r="D30" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="E30" s="93"/>
+      <c r="E30" s="95"/>
       <c r="F30" s="34" t="s">
         <v>33</v>
       </c>
@@ -8945,12 +9041,12 @@
       <c r="K30" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="L30" s="93"/>
-      <c r="M30" s="93"/>
+      <c r="L30" s="95"/>
+      <c r="M30" s="95"/>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
       <c r="P30" s="2"/>
-      <c r="R30" s="93"/>
+      <c r="R30" s="95"/>
       <c r="S30" s="34" t="s">
         <v>13</v>
       </c>
@@ -8960,7 +9056,7 @@
       <c r="U30" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="V30" s="93"/>
+      <c r="V30" s="95"/>
       <c r="W30" s="34" t="s">
         <v>33</v>
       </c>
@@ -8979,8 +9075,8 @@
       <c r="AB30" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="AC30" s="93"/>
-      <c r="AD30" s="93"/>
+      <c r="AC30" s="95"/>
+      <c r="AD30" s="95"/>
       <c r="AE30" s="2"/>
       <c r="AF30" s="2"/>
       <c r="AG30" s="2"/>
@@ -9938,61 +10034,61 @@
       <c r="AG48" s="2"/>
     </row>
     <row r="49" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="92" t="s">
+      <c r="A49" s="94" t="s">
         <v>53</v>
       </c>
-      <c r="B49" s="94" t="s">
+      <c r="B49" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="C49" s="95"/>
-      <c r="D49" s="96"/>
-      <c r="E49" s="92" t="s">
+      <c r="C49" s="100"/>
+      <c r="D49" s="101"/>
+      <c r="E49" s="94" t="s">
         <v>55</v>
       </c>
-      <c r="F49" s="94" t="s">
+      <c r="F49" s="99" t="s">
         <v>56</v>
       </c>
-      <c r="G49" s="95"/>
-      <c r="H49" s="96"/>
-      <c r="I49" s="94" t="s">
+      <c r="G49" s="100"/>
+      <c r="H49" s="101"/>
+      <c r="I49" s="99" t="s">
         <v>57</v>
       </c>
-      <c r="J49" s="95"/>
-      <c r="K49" s="96"/>
-      <c r="L49" s="92" t="s">
+      <c r="J49" s="100"/>
+      <c r="K49" s="101"/>
+      <c r="L49" s="94" t="s">
         <v>58</v>
       </c>
-      <c r="M49" s="92" t="s">
+      <c r="M49" s="94" t="s">
         <v>59</v>
       </c>
       <c r="N49" s="2"/>
       <c r="O49" s="2"/>
       <c r="P49" s="2"/>
-      <c r="R49" s="92" t="s">
+      <c r="R49" s="94" t="s">
         <v>53</v>
       </c>
-      <c r="S49" s="94" t="s">
+      <c r="S49" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="T49" s="95"/>
-      <c r="U49" s="96"/>
-      <c r="V49" s="92" t="s">
+      <c r="T49" s="100"/>
+      <c r="U49" s="101"/>
+      <c r="V49" s="94" t="s">
         <v>55</v>
       </c>
-      <c r="W49" s="94" t="s">
+      <c r="W49" s="99" t="s">
         <v>56</v>
       </c>
-      <c r="X49" s="95"/>
-      <c r="Y49" s="96"/>
-      <c r="Z49" s="94" t="s">
+      <c r="X49" s="100"/>
+      <c r="Y49" s="101"/>
+      <c r="Z49" s="99" t="s">
         <v>57</v>
       </c>
-      <c r="AA49" s="95"/>
-      <c r="AB49" s="96"/>
-      <c r="AC49" s="92" t="s">
+      <c r="AA49" s="100"/>
+      <c r="AB49" s="101"/>
+      <c r="AC49" s="94" t="s">
         <v>58</v>
       </c>
-      <c r="AD49" s="92" t="s">
+      <c r="AD49" s="94" t="s">
         <v>59</v>
       </c>
       <c r="AE49" s="2"/>
@@ -10000,7 +10096,7 @@
       <c r="AG49" s="2"/>
     </row>
     <row r="50" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="93"/>
+      <c r="A50" s="95"/>
       <c r="B50" s="34" t="s">
         <v>13</v>
       </c>
@@ -10010,7 +10106,7 @@
       <c r="D50" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="E50" s="93"/>
+      <c r="E50" s="95"/>
       <c r="F50" s="34" t="s">
         <v>33</v>
       </c>
@@ -10029,12 +10125,12 @@
       <c r="K50" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="L50" s="93"/>
-      <c r="M50" s="93"/>
+      <c r="L50" s="95"/>
+      <c r="M50" s="95"/>
       <c r="N50" s="2"/>
       <c r="O50" s="2"/>
       <c r="P50" s="2"/>
-      <c r="R50" s="93"/>
+      <c r="R50" s="95"/>
       <c r="S50" s="34" t="s">
         <v>13</v>
       </c>
@@ -10044,7 +10140,7 @@
       <c r="U50" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="V50" s="93"/>
+      <c r="V50" s="95"/>
       <c r="W50" s="34" t="s">
         <v>33</v>
       </c>
@@ -10063,8 +10159,8 @@
       <c r="AB50" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="AC50" s="93"/>
-      <c r="AD50" s="93"/>
+      <c r="AC50" s="95"/>
+      <c r="AD50" s="95"/>
       <c r="AE50" s="2"/>
       <c r="AF50" s="2"/>
       <c r="AG50" s="2"/>
@@ -11022,61 +11118,61 @@
       <c r="AG68" s="2"/>
     </row>
     <row r="69" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="92" t="s">
+      <c r="A69" s="94" t="s">
         <v>53</v>
       </c>
-      <c r="B69" s="94" t="s">
+      <c r="B69" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="C69" s="95"/>
-      <c r="D69" s="96"/>
-      <c r="E69" s="92" t="s">
+      <c r="C69" s="100"/>
+      <c r="D69" s="101"/>
+      <c r="E69" s="94" t="s">
         <v>55</v>
       </c>
-      <c r="F69" s="94" t="s">
+      <c r="F69" s="99" t="s">
         <v>56</v>
       </c>
-      <c r="G69" s="95"/>
-      <c r="H69" s="96"/>
-      <c r="I69" s="94" t="s">
+      <c r="G69" s="100"/>
+      <c r="H69" s="101"/>
+      <c r="I69" s="99" t="s">
         <v>57</v>
       </c>
-      <c r="J69" s="95"/>
-      <c r="K69" s="96"/>
-      <c r="L69" s="92" t="s">
+      <c r="J69" s="100"/>
+      <c r="K69" s="101"/>
+      <c r="L69" s="94" t="s">
         <v>58</v>
       </c>
-      <c r="M69" s="92" t="s">
+      <c r="M69" s="94" t="s">
         <v>59</v>
       </c>
       <c r="N69" s="2"/>
       <c r="O69" s="2"/>
       <c r="P69" s="2"/>
-      <c r="R69" s="92" t="s">
+      <c r="R69" s="94" t="s">
         <v>53</v>
       </c>
-      <c r="S69" s="94" t="s">
+      <c r="S69" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="T69" s="95"/>
-      <c r="U69" s="96"/>
-      <c r="V69" s="92" t="s">
+      <c r="T69" s="100"/>
+      <c r="U69" s="101"/>
+      <c r="V69" s="94" t="s">
         <v>55</v>
       </c>
-      <c r="W69" s="94" t="s">
+      <c r="W69" s="99" t="s">
         <v>56</v>
       </c>
-      <c r="X69" s="95"/>
-      <c r="Y69" s="96"/>
-      <c r="Z69" s="94" t="s">
+      <c r="X69" s="100"/>
+      <c r="Y69" s="101"/>
+      <c r="Z69" s="99" t="s">
         <v>57</v>
       </c>
-      <c r="AA69" s="95"/>
-      <c r="AB69" s="96"/>
-      <c r="AC69" s="92" t="s">
+      <c r="AA69" s="100"/>
+      <c r="AB69" s="101"/>
+      <c r="AC69" s="94" t="s">
         <v>58</v>
       </c>
-      <c r="AD69" s="92" t="s">
+      <c r="AD69" s="94" t="s">
         <v>59</v>
       </c>
       <c r="AE69" s="2"/>
@@ -11084,7 +11180,7 @@
       <c r="AG69" s="2"/>
     </row>
     <row r="70" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="93"/>
+      <c r="A70" s="95"/>
       <c r="B70" s="34" t="s">
         <v>13</v>
       </c>
@@ -11094,7 +11190,7 @@
       <c r="D70" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="E70" s="93"/>
+      <c r="E70" s="95"/>
       <c r="F70" s="34" t="s">
         <v>33</v>
       </c>
@@ -11113,12 +11209,12 @@
       <c r="K70" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="L70" s="93"/>
-      <c r="M70" s="93"/>
+      <c r="L70" s="95"/>
+      <c r="M70" s="95"/>
       <c r="N70" s="2"/>
       <c r="O70" s="2"/>
       <c r="P70" s="2"/>
-      <c r="R70" s="93"/>
+      <c r="R70" s="95"/>
       <c r="S70" s="34" t="s">
         <v>13</v>
       </c>
@@ -11128,7 +11224,7 @@
       <c r="U70" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="V70" s="93"/>
+      <c r="V70" s="95"/>
       <c r="W70" s="34" t="s">
         <v>33</v>
       </c>
@@ -11147,8 +11243,8 @@
       <c r="AB70" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="AC70" s="93"/>
-      <c r="AD70" s="93"/>
+      <c r="AC70" s="95"/>
+      <c r="AD70" s="95"/>
       <c r="AE70" s="2"/>
       <c r="AF70" s="2"/>
       <c r="AG70" s="2"/>
@@ -12106,61 +12202,61 @@
       <c r="AG88" s="2"/>
     </row>
     <row r="89" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="92" t="s">
+      <c r="A89" s="94" t="s">
         <v>53</v>
       </c>
-      <c r="B89" s="94" t="s">
+      <c r="B89" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="C89" s="95"/>
-      <c r="D89" s="96"/>
-      <c r="E89" s="92" t="s">
+      <c r="C89" s="100"/>
+      <c r="D89" s="101"/>
+      <c r="E89" s="94" t="s">
         <v>55</v>
       </c>
-      <c r="F89" s="94" t="s">
+      <c r="F89" s="99" t="s">
         <v>56</v>
       </c>
-      <c r="G89" s="95"/>
-      <c r="H89" s="96"/>
-      <c r="I89" s="94" t="s">
+      <c r="G89" s="100"/>
+      <c r="H89" s="101"/>
+      <c r="I89" s="99" t="s">
         <v>57</v>
       </c>
-      <c r="J89" s="95"/>
-      <c r="K89" s="96"/>
-      <c r="L89" s="92" t="s">
+      <c r="J89" s="100"/>
+      <c r="K89" s="101"/>
+      <c r="L89" s="94" t="s">
         <v>58</v>
       </c>
-      <c r="M89" s="92" t="s">
+      <c r="M89" s="94" t="s">
         <v>59</v>
       </c>
       <c r="N89" s="2"/>
       <c r="O89" s="2"/>
       <c r="P89" s="2"/>
-      <c r="R89" s="92" t="s">
+      <c r="R89" s="94" t="s">
         <v>53</v>
       </c>
-      <c r="S89" s="94" t="s">
+      <c r="S89" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="T89" s="95"/>
-      <c r="U89" s="96"/>
-      <c r="V89" s="92" t="s">
+      <c r="T89" s="100"/>
+      <c r="U89" s="101"/>
+      <c r="V89" s="94" t="s">
         <v>55</v>
       </c>
-      <c r="W89" s="94" t="s">
+      <c r="W89" s="99" t="s">
         <v>56</v>
       </c>
-      <c r="X89" s="95"/>
-      <c r="Y89" s="96"/>
-      <c r="Z89" s="94" t="s">
+      <c r="X89" s="100"/>
+      <c r="Y89" s="101"/>
+      <c r="Z89" s="99" t="s">
         <v>57</v>
       </c>
-      <c r="AA89" s="95"/>
-      <c r="AB89" s="96"/>
-      <c r="AC89" s="92" t="s">
+      <c r="AA89" s="100"/>
+      <c r="AB89" s="101"/>
+      <c r="AC89" s="94" t="s">
         <v>58</v>
       </c>
-      <c r="AD89" s="92" t="s">
+      <c r="AD89" s="94" t="s">
         <v>59</v>
       </c>
       <c r="AE89" s="2"/>
@@ -12168,7 +12264,7 @@
       <c r="AG89" s="2"/>
     </row>
     <row r="90" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="93"/>
+      <c r="A90" s="95"/>
       <c r="B90" s="34" t="s">
         <v>13</v>
       </c>
@@ -12178,7 +12274,7 @@
       <c r="D90" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="E90" s="93"/>
+      <c r="E90" s="95"/>
       <c r="F90" s="34" t="s">
         <v>33</v>
       </c>
@@ -12197,12 +12293,12 @@
       <c r="K90" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="L90" s="93"/>
-      <c r="M90" s="93"/>
+      <c r="L90" s="95"/>
+      <c r="M90" s="95"/>
       <c r="N90" s="2"/>
       <c r="O90" s="2"/>
       <c r="P90" s="2"/>
-      <c r="R90" s="93"/>
+      <c r="R90" s="95"/>
       <c r="S90" s="34" t="s">
         <v>13</v>
       </c>
@@ -12212,7 +12308,7 @@
       <c r="U90" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="V90" s="93"/>
+      <c r="V90" s="95"/>
       <c r="W90" s="34" t="s">
         <v>33</v>
       </c>
@@ -12231,8 +12327,8 @@
       <c r="AB90" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="AC90" s="93"/>
-      <c r="AD90" s="93"/>
+      <c r="AC90" s="95"/>
+      <c r="AD90" s="95"/>
       <c r="AE90" s="2"/>
       <c r="AF90" s="2"/>
       <c r="AG90" s="2"/>
@@ -12849,10 +12945,10 @@
     </row>
     <row r="102" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="2"/>
-      <c r="B102" s="97"/>
-      <c r="C102" s="98"/>
-      <c r="D102" s="98"/>
-      <c r="E102" s="99"/>
+      <c r="B102" s="96"/>
+      <c r="C102" s="97"/>
+      <c r="D102" s="97"/>
+      <c r="E102" s="98"/>
       <c r="F102" s="2"/>
       <c r="G102" s="2"/>
       <c r="H102" s="2"/>
@@ -12865,10 +12961,10 @@
       <c r="O102" s="2"/>
       <c r="P102" s="2"/>
       <c r="R102" s="2"/>
-      <c r="S102" s="97"/>
-      <c r="T102" s="98"/>
-      <c r="U102" s="98"/>
-      <c r="V102" s="99"/>
+      <c r="S102" s="96"/>
+      <c r="T102" s="97"/>
+      <c r="U102" s="97"/>
+      <c r="V102" s="98"/>
       <c r="W102" s="2"/>
       <c r="X102" s="2"/>
       <c r="Y102" s="2"/>
@@ -12883,36 +12979,32 @@
     </row>
   </sheetData>
   <mergeCells count="72">
-    <mergeCell ref="AD89:AD90"/>
-    <mergeCell ref="S102:V102"/>
-    <mergeCell ref="R89:R90"/>
-    <mergeCell ref="S89:U89"/>
-    <mergeCell ref="V89:V90"/>
-    <mergeCell ref="W89:Y89"/>
-    <mergeCell ref="Z89:AB89"/>
-    <mergeCell ref="AC89:AC90"/>
-    <mergeCell ref="Z49:AB49"/>
-    <mergeCell ref="AC49:AC50"/>
-    <mergeCell ref="AD49:AD50"/>
-    <mergeCell ref="R69:R70"/>
-    <mergeCell ref="S69:U69"/>
-    <mergeCell ref="V69:V70"/>
-    <mergeCell ref="W69:Y69"/>
-    <mergeCell ref="Z69:AB69"/>
-    <mergeCell ref="AC69:AC70"/>
-    <mergeCell ref="AD69:AD70"/>
-    <mergeCell ref="W49:Y49"/>
-    <mergeCell ref="Z9:AB9"/>
-    <mergeCell ref="AC9:AC10"/>
-    <mergeCell ref="AD9:AD10"/>
-    <mergeCell ref="R29:R30"/>
-    <mergeCell ref="S29:U29"/>
-    <mergeCell ref="V29:V30"/>
-    <mergeCell ref="W29:Y29"/>
-    <mergeCell ref="Z29:AB29"/>
-    <mergeCell ref="AC29:AC30"/>
-    <mergeCell ref="AD29:AD30"/>
-    <mergeCell ref="W9:Y9"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="F49:H49"/>
+    <mergeCell ref="I49:K49"/>
+    <mergeCell ref="A69:A70"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="E69:E70"/>
+    <mergeCell ref="F69:H69"/>
+    <mergeCell ref="I69:K69"/>
+    <mergeCell ref="A89:A90"/>
+    <mergeCell ref="B89:D89"/>
+    <mergeCell ref="E89:E90"/>
+    <mergeCell ref="F89:H89"/>
+    <mergeCell ref="I89:K89"/>
     <mergeCell ref="M89:M90"/>
     <mergeCell ref="B102:E102"/>
     <mergeCell ref="R9:R10"/>
@@ -12929,32 +13021,36 @@
     <mergeCell ref="M9:M10"/>
     <mergeCell ref="L29:L30"/>
     <mergeCell ref="M29:M30"/>
-    <mergeCell ref="A89:A90"/>
-    <mergeCell ref="B89:D89"/>
-    <mergeCell ref="E89:E90"/>
-    <mergeCell ref="F89:H89"/>
-    <mergeCell ref="I89:K89"/>
-    <mergeCell ref="A69:A70"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="E69:E70"/>
-    <mergeCell ref="F69:H69"/>
-    <mergeCell ref="I69:K69"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="F49:H49"/>
-    <mergeCell ref="I49:K49"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="Z9:AB9"/>
+    <mergeCell ref="AC9:AC10"/>
+    <mergeCell ref="AD9:AD10"/>
+    <mergeCell ref="R29:R30"/>
+    <mergeCell ref="S29:U29"/>
+    <mergeCell ref="V29:V30"/>
+    <mergeCell ref="W29:Y29"/>
+    <mergeCell ref="Z29:AB29"/>
+    <mergeCell ref="AC29:AC30"/>
+    <mergeCell ref="AD29:AD30"/>
+    <mergeCell ref="W9:Y9"/>
+    <mergeCell ref="Z49:AB49"/>
+    <mergeCell ref="AC49:AC50"/>
+    <mergeCell ref="AD49:AD50"/>
+    <mergeCell ref="R69:R70"/>
+    <mergeCell ref="S69:U69"/>
+    <mergeCell ref="V69:V70"/>
+    <mergeCell ref="W69:Y69"/>
+    <mergeCell ref="Z69:AB69"/>
+    <mergeCell ref="AC69:AC70"/>
+    <mergeCell ref="AD69:AD70"/>
+    <mergeCell ref="W49:Y49"/>
+    <mergeCell ref="AD89:AD90"/>
+    <mergeCell ref="S102:V102"/>
+    <mergeCell ref="R89:R90"/>
+    <mergeCell ref="S89:U89"/>
+    <mergeCell ref="V89:V90"/>
+    <mergeCell ref="W89:Y89"/>
+    <mergeCell ref="Z89:AB89"/>
+    <mergeCell ref="AC89:AC90"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13096,7 +13192,7 @@
         <v>87</v>
       </c>
       <c r="E7" s="45"/>
-      <c r="H7" s="100" t="s">
+      <c r="H7" s="105" t="s">
         <v>59</v>
       </c>
       <c r="I7" s="50"/>
@@ -13107,7 +13203,7 @@
         <v>88</v>
       </c>
       <c r="L7" s="52"/>
-      <c r="N7" s="102" t="s">
+      <c r="N7" s="107" t="s">
         <v>59</v>
       </c>
       <c r="O7" s="51">
@@ -13116,7 +13212,7 @@
       <c r="P7" t="s">
         <v>88</v>
       </c>
-      <c r="R7" s="102" t="s">
+      <c r="R7" s="107" t="s">
         <v>59</v>
       </c>
       <c r="S7" s="53">
@@ -13135,7 +13231,7 @@
         <v>87</v>
       </c>
       <c r="AA7" s="45"/>
-      <c r="AD7" s="100" t="s">
+      <c r="AD7" s="105" t="s">
         <v>59</v>
       </c>
       <c r="AE7" s="50"/>
@@ -13146,7 +13242,7 @@
         <v>88</v>
       </c>
       <c r="AH7" s="52"/>
-      <c r="AJ7" s="102" t="s">
+      <c r="AJ7" s="107" t="s">
         <v>59</v>
       </c>
       <c r="AK7" s="51">
@@ -13155,7 +13251,7 @@
       <c r="AL7" t="s">
         <v>88</v>
       </c>
-      <c r="AN7" s="102" t="s">
+      <c r="AN7" s="107" t="s">
         <v>59</v>
       </c>
       <c r="AO7" s="53">
@@ -13174,7 +13270,7 @@
       </c>
       <c r="D8" s="54"/>
       <c r="E8" s="54"/>
-      <c r="H8" s="101"/>
+      <c r="H8" s="106"/>
       <c r="I8" s="55"/>
       <c r="J8" s="56">
         <v>1</v>
@@ -13183,14 +13279,14 @@
         <v>89</v>
       </c>
       <c r="L8" s="58"/>
-      <c r="N8" s="102"/>
+      <c r="N8" s="107"/>
       <c r="O8" s="51">
         <v>1</v>
       </c>
       <c r="P8" t="s">
         <v>89</v>
       </c>
-      <c r="R8" s="102"/>
+      <c r="R8" s="107"/>
       <c r="S8" s="53">
         <v>0</v>
       </c>
@@ -13205,7 +13301,7 @@
       </c>
       <c r="Z8" s="54"/>
       <c r="AA8" s="54"/>
-      <c r="AD8" s="101"/>
+      <c r="AD8" s="106"/>
       <c r="AE8" s="55"/>
       <c r="AF8" s="56">
         <v>1</v>
@@ -13214,14 +13310,14 @@
         <v>89</v>
       </c>
       <c r="AH8" s="58"/>
-      <c r="AJ8" s="102"/>
+      <c r="AJ8" s="107"/>
       <c r="AK8" s="51">
         <v>1</v>
       </c>
       <c r="AL8" t="s">
         <v>89</v>
       </c>
-      <c r="AN8" s="102"/>
+      <c r="AN8" s="107"/>
       <c r="AO8" s="53">
         <v>0</v>
       </c>
@@ -13247,7 +13343,7 @@
         <v>52</v>
       </c>
       <c r="P9" s="62"/>
-      <c r="R9" s="102"/>
+      <c r="R9" s="107"/>
       <c r="S9" s="53">
         <v>-1</v>
       </c>
@@ -13271,7 +13367,7 @@
         <v>52</v>
       </c>
       <c r="AL9" s="62"/>
-      <c r="AN9" s="102"/>
+      <c r="AN9" s="107"/>
       <c r="AO9" s="53">
         <v>-1</v>
       </c>
@@ -13280,71 +13376,71 @@
       </c>
     </row>
     <row r="10" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A10" s="103" t="s">
+      <c r="A10" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="105" t="s">
+      <c r="B10" s="108" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="106"/>
-      <c r="D10" s="106"/>
-      <c r="E10" s="107"/>
-      <c r="F10" s="108" t="s">
+      <c r="C10" s="109"/>
+      <c r="D10" s="109"/>
+      <c r="E10" s="110"/>
+      <c r="F10" s="111" t="s">
         <v>93</v>
       </c>
-      <c r="G10" s="110" t="s">
+      <c r="G10" s="113" t="s">
         <v>56</v>
       </c>
-      <c r="H10" s="111"/>
-      <c r="I10" s="111"/>
-      <c r="J10" s="112"/>
-      <c r="K10" s="113" t="s">
+      <c r="H10" s="114"/>
+      <c r="I10" s="114"/>
+      <c r="J10" s="115"/>
+      <c r="K10" s="116" t="s">
         <v>94</v>
       </c>
-      <c r="L10" s="113"/>
-      <c r="M10" s="113"/>
-      <c r="N10" s="113"/>
-      <c r="O10" s="103" t="s">
+      <c r="L10" s="116"/>
+      <c r="M10" s="116"/>
+      <c r="N10" s="116"/>
+      <c r="O10" s="102" t="s">
         <v>58</v>
       </c>
-      <c r="P10" s="103" t="s">
+      <c r="P10" s="102" t="s">
         <v>59</v>
       </c>
       <c r="Q10" s="64"/>
-      <c r="W10" s="103" t="s">
+      <c r="W10" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="X10" s="105" t="s">
+      <c r="X10" s="108" t="s">
         <v>54</v>
       </c>
-      <c r="Y10" s="106"/>
-      <c r="Z10" s="106"/>
-      <c r="AA10" s="107"/>
-      <c r="AB10" s="108" t="s">
+      <c r="Y10" s="109"/>
+      <c r="Z10" s="109"/>
+      <c r="AA10" s="110"/>
+      <c r="AB10" s="111" t="s">
         <v>93</v>
       </c>
-      <c r="AC10" s="110" t="s">
+      <c r="AC10" s="113" t="s">
         <v>56</v>
       </c>
-      <c r="AD10" s="111"/>
-      <c r="AE10" s="111"/>
-      <c r="AF10" s="112"/>
-      <c r="AG10" s="113" t="s">
+      <c r="AD10" s="114"/>
+      <c r="AE10" s="114"/>
+      <c r="AF10" s="115"/>
+      <c r="AG10" s="116" t="s">
         <v>94</v>
       </c>
-      <c r="AH10" s="113"/>
-      <c r="AI10" s="113"/>
-      <c r="AJ10" s="113"/>
-      <c r="AK10" s="103" t="s">
+      <c r="AH10" s="116"/>
+      <c r="AI10" s="116"/>
+      <c r="AJ10" s="116"/>
+      <c r="AK10" s="102" t="s">
         <v>58</v>
       </c>
-      <c r="AL10" s="103" t="s">
+      <c r="AL10" s="102" t="s">
         <v>59</v>
       </c>
       <c r="AM10" s="64"/>
     </row>
     <row r="11" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A11" s="104"/>
+      <c r="A11" s="103"/>
       <c r="B11" s="63" t="s">
         <v>13</v>
       </c>
@@ -13357,7 +13453,7 @@
       <c r="E11" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="F11" s="109"/>
+      <c r="F11" s="112"/>
       <c r="G11" s="65" t="s">
         <v>33</v>
       </c>
@@ -13382,9 +13478,9 @@
       <c r="N11" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="O11" s="104"/>
-      <c r="P11" s="104"/>
-      <c r="W11" s="104"/>
+      <c r="O11" s="103"/>
+      <c r="P11" s="103"/>
+      <c r="W11" s="103"/>
       <c r="X11" s="63" t="s">
         <v>13</v>
       </c>
@@ -13397,7 +13493,7 @@
       <c r="AA11" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="AB11" s="109"/>
+      <c r="AB11" s="112"/>
       <c r="AC11" s="65" t="s">
         <v>33</v>
       </c>
@@ -13422,8 +13518,8 @@
       <c r="AJ11" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="AK11" s="104"/>
-      <c r="AL11" s="104"/>
+      <c r="AK11" s="103"/>
+      <c r="AL11" s="103"/>
     </row>
     <row r="12" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A12" s="66">
@@ -14373,21 +14469,21 @@
       <c r="A20" t="s">
         <v>98</v>
       </c>
-      <c r="K20" s="114" t="s">
+      <c r="K20" s="104" t="s">
         <v>99</v>
       </c>
-      <c r="L20" s="114"/>
-      <c r="M20" s="114"/>
-      <c r="N20" s="114"/>
+      <c r="L20" s="104"/>
+      <c r="M20" s="104"/>
+      <c r="N20" s="104"/>
       <c r="W20" t="s">
         <v>98</v>
       </c>
-      <c r="AG20" s="114" t="s">
+      <c r="AG20" s="104" t="s">
         <v>99</v>
       </c>
-      <c r="AH20" s="114"/>
-      <c r="AI20" s="114"/>
-      <c r="AJ20" s="114"/>
+      <c r="AH20" s="104"/>
+      <c r="AI20" s="104"/>
+      <c r="AJ20" s="104"/>
     </row>
     <row r="21" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -14523,7 +14619,7 @@
         <v>87</v>
       </c>
       <c r="E31" s="45"/>
-      <c r="H31" s="100" t="s">
+      <c r="H31" s="105" t="s">
         <v>59</v>
       </c>
       <c r="I31" s="50"/>
@@ -14534,7 +14630,7 @@
         <v>88</v>
       </c>
       <c r="L31" s="52"/>
-      <c r="N31" s="102" t="s">
+      <c r="N31" s="107" t="s">
         <v>59</v>
       </c>
       <c r="O31" s="51">
@@ -14543,7 +14639,7 @@
       <c r="P31" t="s">
         <v>88</v>
       </c>
-      <c r="R31" s="102" t="s">
+      <c r="R31" s="107" t="s">
         <v>59</v>
       </c>
       <c r="S31" s="53">
@@ -14562,7 +14658,7 @@
         <v>87</v>
       </c>
       <c r="AA31" s="45"/>
-      <c r="AD31" s="100" t="s">
+      <c r="AD31" s="105" t="s">
         <v>59</v>
       </c>
       <c r="AE31" s="50"/>
@@ -14573,7 +14669,7 @@
         <v>88</v>
       </c>
       <c r="AH31" s="52"/>
-      <c r="AJ31" s="102" t="s">
+      <c r="AJ31" s="107" t="s">
         <v>59</v>
       </c>
       <c r="AK31" s="51">
@@ -14582,7 +14678,7 @@
       <c r="AL31" t="s">
         <v>88</v>
       </c>
-      <c r="AN31" s="102" t="s">
+      <c r="AN31" s="107" t="s">
         <v>59</v>
       </c>
       <c r="AO31" s="53">
@@ -14601,7 +14697,7 @@
       </c>
       <c r="D32" s="54"/>
       <c r="E32" s="54"/>
-      <c r="H32" s="101"/>
+      <c r="H32" s="106"/>
       <c r="I32" s="55"/>
       <c r="J32" s="56">
         <v>1</v>
@@ -14610,14 +14706,14 @@
         <v>89</v>
       </c>
       <c r="L32" s="58"/>
-      <c r="N32" s="102"/>
+      <c r="N32" s="107"/>
       <c r="O32" s="51">
         <v>1</v>
       </c>
       <c r="P32" t="s">
         <v>89</v>
       </c>
-      <c r="R32" s="102"/>
+      <c r="R32" s="107"/>
       <c r="S32" s="53">
         <v>0</v>
       </c>
@@ -14632,7 +14728,7 @@
       </c>
       <c r="Z32" s="54"/>
       <c r="AA32" s="54"/>
-      <c r="AD32" s="101"/>
+      <c r="AD32" s="106"/>
       <c r="AE32" s="55"/>
       <c r="AF32" s="56">
         <v>1</v>
@@ -14641,14 +14737,14 @@
         <v>89</v>
       </c>
       <c r="AH32" s="58"/>
-      <c r="AJ32" s="102"/>
+      <c r="AJ32" s="107"/>
       <c r="AK32" s="51">
         <v>1</v>
       </c>
       <c r="AL32" t="s">
         <v>89</v>
       </c>
-      <c r="AN32" s="102"/>
+      <c r="AN32" s="107"/>
       <c r="AO32" s="53">
         <v>0</v>
       </c>
@@ -14674,7 +14770,7 @@
         <v>52</v>
       </c>
       <c r="P33" s="62"/>
-      <c r="R33" s="102"/>
+      <c r="R33" s="107"/>
       <c r="S33" s="53">
         <v>-1</v>
       </c>
@@ -14698,7 +14794,7 @@
         <v>52</v>
       </c>
       <c r="AL33" s="62"/>
-      <c r="AN33" s="102"/>
+      <c r="AN33" s="107"/>
       <c r="AO33" s="53">
         <v>-1</v>
       </c>
@@ -14707,71 +14803,71 @@
       </c>
     </row>
     <row r="34" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A34" s="103" t="s">
+      <c r="A34" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="105" t="s">
+      <c r="B34" s="108" t="s">
         <v>54</v>
       </c>
-      <c r="C34" s="106"/>
-      <c r="D34" s="106"/>
-      <c r="E34" s="107"/>
-      <c r="F34" s="108" t="s">
+      <c r="C34" s="109"/>
+      <c r="D34" s="109"/>
+      <c r="E34" s="110"/>
+      <c r="F34" s="111" t="s">
         <v>93</v>
       </c>
-      <c r="G34" s="110" t="s">
+      <c r="G34" s="113" t="s">
         <v>56</v>
       </c>
-      <c r="H34" s="111"/>
-      <c r="I34" s="111"/>
-      <c r="J34" s="112"/>
-      <c r="K34" s="113" t="s">
+      <c r="H34" s="114"/>
+      <c r="I34" s="114"/>
+      <c r="J34" s="115"/>
+      <c r="K34" s="116" t="s">
         <v>94</v>
       </c>
-      <c r="L34" s="113"/>
-      <c r="M34" s="113"/>
-      <c r="N34" s="113"/>
-      <c r="O34" s="103" t="s">
+      <c r="L34" s="116"/>
+      <c r="M34" s="116"/>
+      <c r="N34" s="116"/>
+      <c r="O34" s="102" t="s">
         <v>58</v>
       </c>
-      <c r="P34" s="103" t="s">
+      <c r="P34" s="102" t="s">
         <v>59</v>
       </c>
       <c r="Q34" s="64"/>
-      <c r="W34" s="103" t="s">
+      <c r="W34" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="X34" s="105" t="s">
+      <c r="X34" s="108" t="s">
         <v>54</v>
       </c>
-      <c r="Y34" s="106"/>
-      <c r="Z34" s="106"/>
-      <c r="AA34" s="107"/>
-      <c r="AB34" s="108" t="s">
+      <c r="Y34" s="109"/>
+      <c r="Z34" s="109"/>
+      <c r="AA34" s="110"/>
+      <c r="AB34" s="111" t="s">
         <v>93</v>
       </c>
-      <c r="AC34" s="110" t="s">
+      <c r="AC34" s="113" t="s">
         <v>56</v>
       </c>
-      <c r="AD34" s="111"/>
-      <c r="AE34" s="111"/>
-      <c r="AF34" s="112"/>
-      <c r="AG34" s="113" t="s">
+      <c r="AD34" s="114"/>
+      <c r="AE34" s="114"/>
+      <c r="AF34" s="115"/>
+      <c r="AG34" s="116" t="s">
         <v>94</v>
       </c>
-      <c r="AH34" s="113"/>
-      <c r="AI34" s="113"/>
-      <c r="AJ34" s="113"/>
-      <c r="AK34" s="103" t="s">
+      <c r="AH34" s="116"/>
+      <c r="AI34" s="116"/>
+      <c r="AJ34" s="116"/>
+      <c r="AK34" s="102" t="s">
         <v>58</v>
       </c>
-      <c r="AL34" s="103" t="s">
+      <c r="AL34" s="102" t="s">
         <v>59</v>
       </c>
       <c r="AM34" s="64"/>
     </row>
     <row r="35" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A35" s="104"/>
+      <c r="A35" s="103"/>
       <c r="B35" s="63" t="s">
         <v>13</v>
       </c>
@@ -14784,7 +14880,7 @@
       <c r="E35" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="F35" s="109"/>
+      <c r="F35" s="112"/>
       <c r="G35" s="65" t="s">
         <v>33</v>
       </c>
@@ -14809,9 +14905,9 @@
       <c r="N35" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="O35" s="104"/>
-      <c r="P35" s="104"/>
-      <c r="W35" s="104"/>
+      <c r="O35" s="103"/>
+      <c r="P35" s="103"/>
+      <c r="W35" s="103"/>
       <c r="X35" s="63" t="s">
         <v>13</v>
       </c>
@@ -14824,7 +14920,7 @@
       <c r="AA35" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="AB35" s="109"/>
+      <c r="AB35" s="112"/>
       <c r="AC35" s="65" t="s">
         <v>33</v>
       </c>
@@ -14849,8 +14945,8 @@
       <c r="AJ35" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="AK35" s="104"/>
-      <c r="AL35" s="104"/>
+      <c r="AK35" s="103"/>
+      <c r="AL35" s="103"/>
     </row>
     <row r="36" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A36" s="66">
@@ -15800,21 +15896,21 @@
       <c r="A44" t="s">
         <v>98</v>
       </c>
-      <c r="K44" s="114" t="s">
+      <c r="K44" s="104" t="s">
         <v>99</v>
       </c>
-      <c r="L44" s="114"/>
-      <c r="M44" s="114"/>
-      <c r="N44" s="114"/>
+      <c r="L44" s="104"/>
+      <c r="M44" s="104"/>
+      <c r="N44" s="104"/>
       <c r="W44" t="s">
         <v>98</v>
       </c>
-      <c r="AG44" s="114" t="s">
+      <c r="AG44" s="104" t="s">
         <v>99</v>
       </c>
-      <c r="AH44" s="114"/>
-      <c r="AI44" s="114"/>
-      <c r="AJ44" s="114"/>
+      <c r="AH44" s="104"/>
+      <c r="AI44" s="104"/>
+      <c r="AJ44" s="104"/>
     </row>
     <row r="45" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
@@ -15941,7 +16037,7 @@
         <v>87</v>
       </c>
       <c r="E55" s="45"/>
-      <c r="H55" s="100" t="s">
+      <c r="H55" s="105" t="s">
         <v>59</v>
       </c>
       <c r="I55" s="50"/>
@@ -15952,7 +16048,7 @@
         <v>88</v>
       </c>
       <c r="L55" s="52"/>
-      <c r="N55" s="102" t="s">
+      <c r="N55" s="107" t="s">
         <v>59</v>
       </c>
       <c r="O55" s="51">
@@ -15961,7 +16057,7 @@
       <c r="P55" t="s">
         <v>88</v>
       </c>
-      <c r="R55" s="102" t="s">
+      <c r="R55" s="107" t="s">
         <v>59</v>
       </c>
       <c r="S55" s="53">
@@ -15980,7 +16076,7 @@
         <v>87</v>
       </c>
       <c r="AA55" s="45"/>
-      <c r="AD55" s="100" t="s">
+      <c r="AD55" s="105" t="s">
         <v>59</v>
       </c>
       <c r="AE55" s="50"/>
@@ -15991,7 +16087,7 @@
         <v>88</v>
       </c>
       <c r="AH55" s="52"/>
-      <c r="AJ55" s="102" t="s">
+      <c r="AJ55" s="107" t="s">
         <v>59</v>
       </c>
       <c r="AK55" s="51">
@@ -16000,7 +16096,7 @@
       <c r="AL55" t="s">
         <v>88</v>
       </c>
-      <c r="AN55" s="102" t="s">
+      <c r="AN55" s="107" t="s">
         <v>59</v>
       </c>
       <c r="AO55" s="53">
@@ -16019,7 +16115,7 @@
       </c>
       <c r="D56" s="54"/>
       <c r="E56" s="54"/>
-      <c r="H56" s="101"/>
+      <c r="H56" s="106"/>
       <c r="I56" s="55"/>
       <c r="J56" s="56">
         <v>1</v>
@@ -16028,14 +16124,14 @@
         <v>89</v>
       </c>
       <c r="L56" s="58"/>
-      <c r="N56" s="102"/>
+      <c r="N56" s="107"/>
       <c r="O56" s="51">
         <v>1</v>
       </c>
       <c r="P56" t="s">
         <v>89</v>
       </c>
-      <c r="R56" s="102"/>
+      <c r="R56" s="107"/>
       <c r="S56" s="53">
         <v>0</v>
       </c>
@@ -16050,7 +16146,7 @@
       </c>
       <c r="Z56" s="54"/>
       <c r="AA56" s="54"/>
-      <c r="AD56" s="101"/>
+      <c r="AD56" s="106"/>
       <c r="AE56" s="55"/>
       <c r="AF56" s="56">
         <v>1</v>
@@ -16059,14 +16155,14 @@
         <v>89</v>
       </c>
       <c r="AH56" s="58"/>
-      <c r="AJ56" s="102"/>
+      <c r="AJ56" s="107"/>
       <c r="AK56" s="51">
         <v>1</v>
       </c>
       <c r="AL56" t="s">
         <v>89</v>
       </c>
-      <c r="AN56" s="102"/>
+      <c r="AN56" s="107"/>
       <c r="AO56" s="53">
         <v>0</v>
       </c>
@@ -16092,7 +16188,7 @@
         <v>52</v>
       </c>
       <c r="P57" s="62"/>
-      <c r="R57" s="102"/>
+      <c r="R57" s="107"/>
       <c r="S57" s="53">
         <v>-1</v>
       </c>
@@ -16116,7 +16212,7 @@
         <v>52</v>
       </c>
       <c r="AL57" s="62"/>
-      <c r="AN57" s="102"/>
+      <c r="AN57" s="107"/>
       <c r="AO57" s="53">
         <v>-1</v>
       </c>
@@ -16125,71 +16221,71 @@
       </c>
     </row>
     <row r="58" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A58" s="103" t="s">
+      <c r="A58" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="B58" s="105" t="s">
+      <c r="B58" s="108" t="s">
         <v>54</v>
       </c>
-      <c r="C58" s="106"/>
-      <c r="D58" s="106"/>
-      <c r="E58" s="107"/>
-      <c r="F58" s="108" t="s">
+      <c r="C58" s="109"/>
+      <c r="D58" s="109"/>
+      <c r="E58" s="110"/>
+      <c r="F58" s="111" t="s">
         <v>93</v>
       </c>
-      <c r="G58" s="110" t="s">
+      <c r="G58" s="113" t="s">
         <v>56</v>
       </c>
-      <c r="H58" s="111"/>
-      <c r="I58" s="111"/>
-      <c r="J58" s="112"/>
-      <c r="K58" s="113" t="s">
+      <c r="H58" s="114"/>
+      <c r="I58" s="114"/>
+      <c r="J58" s="115"/>
+      <c r="K58" s="116" t="s">
         <v>94</v>
       </c>
-      <c r="L58" s="113"/>
-      <c r="M58" s="113"/>
-      <c r="N58" s="113"/>
-      <c r="O58" s="103" t="s">
+      <c r="L58" s="116"/>
+      <c r="M58" s="116"/>
+      <c r="N58" s="116"/>
+      <c r="O58" s="102" t="s">
         <v>58</v>
       </c>
-      <c r="P58" s="103" t="s">
+      <c r="P58" s="102" t="s">
         <v>59</v>
       </c>
       <c r="Q58" s="64"/>
-      <c r="W58" s="103" t="s">
+      <c r="W58" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="X58" s="105" t="s">
+      <c r="X58" s="108" t="s">
         <v>54</v>
       </c>
-      <c r="Y58" s="106"/>
-      <c r="Z58" s="106"/>
-      <c r="AA58" s="107"/>
-      <c r="AB58" s="108" t="s">
+      <c r="Y58" s="109"/>
+      <c r="Z58" s="109"/>
+      <c r="AA58" s="110"/>
+      <c r="AB58" s="111" t="s">
         <v>93</v>
       </c>
-      <c r="AC58" s="110" t="s">
+      <c r="AC58" s="113" t="s">
         <v>56</v>
       </c>
-      <c r="AD58" s="111"/>
-      <c r="AE58" s="111"/>
-      <c r="AF58" s="112"/>
-      <c r="AG58" s="113" t="s">
+      <c r="AD58" s="114"/>
+      <c r="AE58" s="114"/>
+      <c r="AF58" s="115"/>
+      <c r="AG58" s="116" t="s">
         <v>94</v>
       </c>
-      <c r="AH58" s="113"/>
-      <c r="AI58" s="113"/>
-      <c r="AJ58" s="113"/>
-      <c r="AK58" s="103" t="s">
+      <c r="AH58" s="116"/>
+      <c r="AI58" s="116"/>
+      <c r="AJ58" s="116"/>
+      <c r="AK58" s="102" t="s">
         <v>58</v>
       </c>
-      <c r="AL58" s="103" t="s">
+      <c r="AL58" s="102" t="s">
         <v>59</v>
       </c>
       <c r="AM58" s="64"/>
     </row>
     <row r="59" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A59" s="104"/>
+      <c r="A59" s="103"/>
       <c r="B59" s="63" t="s">
         <v>13</v>
       </c>
@@ -16202,7 +16298,7 @@
       <c r="E59" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="F59" s="109"/>
+      <c r="F59" s="112"/>
       <c r="G59" s="65" t="s">
         <v>33</v>
       </c>
@@ -16227,9 +16323,9 @@
       <c r="N59" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="O59" s="104"/>
-      <c r="P59" s="104"/>
-      <c r="W59" s="104"/>
+      <c r="O59" s="103"/>
+      <c r="P59" s="103"/>
+      <c r="W59" s="103"/>
       <c r="X59" s="63" t="s">
         <v>13</v>
       </c>
@@ -16242,7 +16338,7 @@
       <c r="AA59" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="AB59" s="109"/>
+      <c r="AB59" s="112"/>
       <c r="AC59" s="65" t="s">
         <v>33</v>
       </c>
@@ -16267,8 +16363,8 @@
       <c r="AJ59" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="AK59" s="104"/>
-      <c r="AL59" s="104"/>
+      <c r="AK59" s="103"/>
+      <c r="AL59" s="103"/>
     </row>
     <row r="60" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A60" s="66">
@@ -17218,21 +17314,21 @@
       <c r="A68" t="s">
         <v>98</v>
       </c>
-      <c r="K68" s="114" t="s">
+      <c r="K68" s="104" t="s">
         <v>99</v>
       </c>
-      <c r="L68" s="114"/>
-      <c r="M68" s="114"/>
-      <c r="N68" s="114"/>
+      <c r="L68" s="104"/>
+      <c r="M68" s="104"/>
+      <c r="N68" s="104"/>
       <c r="W68" t="s">
         <v>98</v>
       </c>
-      <c r="AG68" s="114" t="s">
+      <c r="AG68" s="104" t="s">
         <v>99</v>
       </c>
-      <c r="AH68" s="114"/>
-      <c r="AI68" s="114"/>
-      <c r="AJ68" s="114"/>
+      <c r="AH68" s="104"/>
+      <c r="AI68" s="104"/>
+      <c r="AJ68" s="104"/>
     </row>
     <row r="69" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
@@ -17359,7 +17455,7 @@
         <v>87</v>
       </c>
       <c r="E78" s="45"/>
-      <c r="H78" s="100" t="s">
+      <c r="H78" s="105" t="s">
         <v>59</v>
       </c>
       <c r="I78" s="50"/>
@@ -17370,7 +17466,7 @@
         <v>88</v>
       </c>
       <c r="L78" s="52"/>
-      <c r="N78" s="102" t="s">
+      <c r="N78" s="107" t="s">
         <v>59</v>
       </c>
       <c r="O78" s="51">
@@ -17379,7 +17475,7 @@
       <c r="P78" t="s">
         <v>88</v>
       </c>
-      <c r="R78" s="102" t="s">
+      <c r="R78" s="107" t="s">
         <v>59</v>
       </c>
       <c r="S78" s="53">
@@ -17398,7 +17494,7 @@
         <v>87</v>
       </c>
       <c r="AA78" s="45"/>
-      <c r="AD78" s="100" t="s">
+      <c r="AD78" s="105" t="s">
         <v>59</v>
       </c>
       <c r="AE78" s="50"/>
@@ -17409,7 +17505,7 @@
         <v>88</v>
       </c>
       <c r="AH78" s="52"/>
-      <c r="AJ78" s="102" t="s">
+      <c r="AJ78" s="107" t="s">
         <v>59</v>
       </c>
       <c r="AK78" s="51">
@@ -17418,7 +17514,7 @@
       <c r="AL78" t="s">
         <v>88</v>
       </c>
-      <c r="AN78" s="102" t="s">
+      <c r="AN78" s="107" t="s">
         <v>59</v>
       </c>
       <c r="AO78" s="53">
@@ -17437,7 +17533,7 @@
       </c>
       <c r="D79" s="54"/>
       <c r="E79" s="54"/>
-      <c r="H79" s="101"/>
+      <c r="H79" s="106"/>
       <c r="I79" s="55"/>
       <c r="J79" s="56">
         <v>1</v>
@@ -17446,14 +17542,14 @@
         <v>89</v>
       </c>
       <c r="L79" s="58"/>
-      <c r="N79" s="102"/>
+      <c r="N79" s="107"/>
       <c r="O79" s="51">
         <v>1</v>
       </c>
       <c r="P79" t="s">
         <v>89</v>
       </c>
-      <c r="R79" s="102"/>
+      <c r="R79" s="107"/>
       <c r="S79" s="53">
         <v>0</v>
       </c>
@@ -17468,7 +17564,7 @@
       </c>
       <c r="Z79" s="54"/>
       <c r="AA79" s="54"/>
-      <c r="AD79" s="101"/>
+      <c r="AD79" s="106"/>
       <c r="AE79" s="55"/>
       <c r="AF79" s="56">
         <v>1</v>
@@ -17477,14 +17573,14 @@
         <v>89</v>
       </c>
       <c r="AH79" s="58"/>
-      <c r="AJ79" s="102"/>
+      <c r="AJ79" s="107"/>
       <c r="AK79" s="51">
         <v>1</v>
       </c>
       <c r="AL79" t="s">
         <v>89</v>
       </c>
-      <c r="AN79" s="102"/>
+      <c r="AN79" s="107"/>
       <c r="AO79" s="53">
         <v>0</v>
       </c>
@@ -17510,7 +17606,7 @@
         <v>52</v>
       </c>
       <c r="P80" s="62"/>
-      <c r="R80" s="102"/>
+      <c r="R80" s="107"/>
       <c r="S80" s="53">
         <v>-1</v>
       </c>
@@ -17534,7 +17630,7 @@
         <v>52</v>
       </c>
       <c r="AL80" s="62"/>
-      <c r="AN80" s="102"/>
+      <c r="AN80" s="107"/>
       <c r="AO80" s="53">
         <v>-1</v>
       </c>
@@ -17543,71 +17639,71 @@
       </c>
     </row>
     <row r="81" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A81" s="103" t="s">
+      <c r="A81" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="B81" s="105" t="s">
+      <c r="B81" s="108" t="s">
         <v>54</v>
       </c>
-      <c r="C81" s="106"/>
-      <c r="D81" s="106"/>
-      <c r="E81" s="107"/>
-      <c r="F81" s="108" t="s">
+      <c r="C81" s="109"/>
+      <c r="D81" s="109"/>
+      <c r="E81" s="110"/>
+      <c r="F81" s="111" t="s">
         <v>93</v>
       </c>
-      <c r="G81" s="110" t="s">
+      <c r="G81" s="113" t="s">
         <v>56</v>
       </c>
-      <c r="H81" s="111"/>
-      <c r="I81" s="111"/>
-      <c r="J81" s="112"/>
-      <c r="K81" s="113" t="s">
+      <c r="H81" s="114"/>
+      <c r="I81" s="114"/>
+      <c r="J81" s="115"/>
+      <c r="K81" s="116" t="s">
         <v>94</v>
       </c>
-      <c r="L81" s="113"/>
-      <c r="M81" s="113"/>
-      <c r="N81" s="113"/>
-      <c r="O81" s="103" t="s">
+      <c r="L81" s="116"/>
+      <c r="M81" s="116"/>
+      <c r="N81" s="116"/>
+      <c r="O81" s="102" t="s">
         <v>58</v>
       </c>
-      <c r="P81" s="103" t="s">
+      <c r="P81" s="102" t="s">
         <v>59</v>
       </c>
       <c r="Q81" s="64"/>
-      <c r="W81" s="103" t="s">
+      <c r="W81" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="X81" s="105" t="s">
+      <c r="X81" s="108" t="s">
         <v>54</v>
       </c>
-      <c r="Y81" s="106"/>
-      <c r="Z81" s="106"/>
-      <c r="AA81" s="107"/>
-      <c r="AB81" s="108" t="s">
+      <c r="Y81" s="109"/>
+      <c r="Z81" s="109"/>
+      <c r="AA81" s="110"/>
+      <c r="AB81" s="111" t="s">
         <v>93</v>
       </c>
-      <c r="AC81" s="110" t="s">
+      <c r="AC81" s="113" t="s">
         <v>56</v>
       </c>
-      <c r="AD81" s="111"/>
-      <c r="AE81" s="111"/>
-      <c r="AF81" s="112"/>
-      <c r="AG81" s="113" t="s">
+      <c r="AD81" s="114"/>
+      <c r="AE81" s="114"/>
+      <c r="AF81" s="115"/>
+      <c r="AG81" s="116" t="s">
         <v>94</v>
       </c>
-      <c r="AH81" s="113"/>
-      <c r="AI81" s="113"/>
-      <c r="AJ81" s="113"/>
-      <c r="AK81" s="103" t="s">
+      <c r="AH81" s="116"/>
+      <c r="AI81" s="116"/>
+      <c r="AJ81" s="116"/>
+      <c r="AK81" s="102" t="s">
         <v>58</v>
       </c>
-      <c r="AL81" s="103" t="s">
+      <c r="AL81" s="102" t="s">
         <v>59</v>
       </c>
       <c r="AM81" s="64"/>
     </row>
     <row r="82" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A82" s="104"/>
+      <c r="A82" s="103"/>
       <c r="B82" s="63" t="s">
         <v>13</v>
       </c>
@@ -17620,7 +17716,7 @@
       <c r="E82" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="F82" s="109"/>
+      <c r="F82" s="112"/>
       <c r="G82" s="65" t="s">
         <v>33</v>
       </c>
@@ -17645,9 +17741,9 @@
       <c r="N82" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="O82" s="104"/>
-      <c r="P82" s="104"/>
-      <c r="W82" s="104"/>
+      <c r="O82" s="103"/>
+      <c r="P82" s="103"/>
+      <c r="W82" s="103"/>
       <c r="X82" s="63" t="s">
         <v>13</v>
       </c>
@@ -17660,7 +17756,7 @@
       <c r="AA82" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="AB82" s="109"/>
+      <c r="AB82" s="112"/>
       <c r="AC82" s="65" t="s">
         <v>33</v>
       </c>
@@ -17685,8 +17781,8 @@
       <c r="AJ82" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="AK82" s="104"/>
-      <c r="AL82" s="104"/>
+      <c r="AK82" s="103"/>
+      <c r="AL82" s="103"/>
     </row>
     <row r="83" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A83" s="66">
@@ -18636,21 +18732,21 @@
       <c r="A91" t="s">
         <v>98</v>
       </c>
-      <c r="K91" s="114" t="s">
+      <c r="K91" s="104" t="s">
         <v>99</v>
       </c>
-      <c r="L91" s="114"/>
-      <c r="M91" s="114"/>
-      <c r="N91" s="114"/>
+      <c r="L91" s="104"/>
+      <c r="M91" s="104"/>
+      <c r="N91" s="104"/>
       <c r="W91" t="s">
         <v>98</v>
       </c>
-      <c r="AG91" s="114" t="s">
+      <c r="AG91" s="104" t="s">
         <v>99</v>
       </c>
-      <c r="AH91" s="114"/>
-      <c r="AI91" s="114"/>
-      <c r="AJ91" s="114"/>
+      <c r="AH91" s="104"/>
+      <c r="AI91" s="104"/>
+      <c r="AJ91" s="104"/>
     </row>
     <row r="92" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
@@ -18777,7 +18873,7 @@
         <v>87</v>
       </c>
       <c r="E101" s="45"/>
-      <c r="H101" s="100" t="s">
+      <c r="H101" s="105" t="s">
         <v>59</v>
       </c>
       <c r="I101" s="50"/>
@@ -18788,7 +18884,7 @@
         <v>88</v>
       </c>
       <c r="L101" s="52"/>
-      <c r="N101" s="102" t="s">
+      <c r="N101" s="107" t="s">
         <v>59</v>
       </c>
       <c r="O101" s="51">
@@ -18797,7 +18893,7 @@
       <c r="P101" t="s">
         <v>88</v>
       </c>
-      <c r="R101" s="102" t="s">
+      <c r="R101" s="107" t="s">
         <v>59</v>
       </c>
       <c r="S101" s="53">
@@ -18816,7 +18912,7 @@
         <v>87</v>
       </c>
       <c r="AA101" s="45"/>
-      <c r="AD101" s="100" t="s">
+      <c r="AD101" s="105" t="s">
         <v>59</v>
       </c>
       <c r="AE101" s="50"/>
@@ -18827,7 +18923,7 @@
         <v>88</v>
       </c>
       <c r="AH101" s="52"/>
-      <c r="AJ101" s="102" t="s">
+      <c r="AJ101" s="107" t="s">
         <v>59</v>
       </c>
       <c r="AK101" s="51">
@@ -18836,7 +18932,7 @@
       <c r="AL101" t="s">
         <v>88</v>
       </c>
-      <c r="AN101" s="102" t="s">
+      <c r="AN101" s="107" t="s">
         <v>59</v>
       </c>
       <c r="AO101" s="53">
@@ -18855,7 +18951,7 @@
       </c>
       <c r="D102" s="54"/>
       <c r="E102" s="54"/>
-      <c r="H102" s="101"/>
+      <c r="H102" s="106"/>
       <c r="I102" s="55"/>
       <c r="J102" s="56">
         <v>1</v>
@@ -18864,14 +18960,14 @@
         <v>89</v>
       </c>
       <c r="L102" s="58"/>
-      <c r="N102" s="102"/>
+      <c r="N102" s="107"/>
       <c r="O102" s="51">
         <v>1</v>
       </c>
       <c r="P102" t="s">
         <v>89</v>
       </c>
-      <c r="R102" s="102"/>
+      <c r="R102" s="107"/>
       <c r="S102" s="53">
         <v>0</v>
       </c>
@@ -18886,7 +18982,7 @@
       </c>
       <c r="Z102" s="54"/>
       <c r="AA102" s="54"/>
-      <c r="AD102" s="101"/>
+      <c r="AD102" s="106"/>
       <c r="AE102" s="55"/>
       <c r="AF102" s="56">
         <v>1</v>
@@ -18895,14 +18991,14 @@
         <v>89</v>
       </c>
       <c r="AH102" s="58"/>
-      <c r="AJ102" s="102"/>
+      <c r="AJ102" s="107"/>
       <c r="AK102" s="51">
         <v>1</v>
       </c>
       <c r="AL102" t="s">
         <v>89</v>
       </c>
-      <c r="AN102" s="102"/>
+      <c r="AN102" s="107"/>
       <c r="AO102" s="53">
         <v>0</v>
       </c>
@@ -18928,7 +19024,7 @@
         <v>52</v>
       </c>
       <c r="P103" s="62"/>
-      <c r="R103" s="102"/>
+      <c r="R103" s="107"/>
       <c r="S103" s="53">
         <v>-1</v>
       </c>
@@ -18952,7 +19048,7 @@
         <v>52</v>
       </c>
       <c r="AL103" s="62"/>
-      <c r="AN103" s="102"/>
+      <c r="AN103" s="107"/>
       <c r="AO103" s="53">
         <v>-1</v>
       </c>
@@ -18961,71 +19057,71 @@
       </c>
     </row>
     <row r="104" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A104" s="103" t="s">
+      <c r="A104" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="B104" s="105" t="s">
+      <c r="B104" s="108" t="s">
         <v>54</v>
       </c>
-      <c r="C104" s="106"/>
-      <c r="D104" s="106"/>
-      <c r="E104" s="107"/>
-      <c r="F104" s="108" t="s">
+      <c r="C104" s="109"/>
+      <c r="D104" s="109"/>
+      <c r="E104" s="110"/>
+      <c r="F104" s="111" t="s">
         <v>93</v>
       </c>
-      <c r="G104" s="110" t="s">
+      <c r="G104" s="113" t="s">
         <v>56</v>
       </c>
-      <c r="H104" s="111"/>
-      <c r="I104" s="111"/>
-      <c r="J104" s="112"/>
-      <c r="K104" s="113" t="s">
+      <c r="H104" s="114"/>
+      <c r="I104" s="114"/>
+      <c r="J104" s="115"/>
+      <c r="K104" s="116" t="s">
         <v>94</v>
       </c>
-      <c r="L104" s="113"/>
-      <c r="M104" s="113"/>
-      <c r="N104" s="113"/>
-      <c r="O104" s="103" t="s">
+      <c r="L104" s="116"/>
+      <c r="M104" s="116"/>
+      <c r="N104" s="116"/>
+      <c r="O104" s="102" t="s">
         <v>58</v>
       </c>
-      <c r="P104" s="103" t="s">
+      <c r="P104" s="102" t="s">
         <v>59</v>
       </c>
       <c r="Q104" s="64"/>
-      <c r="W104" s="103" t="s">
+      <c r="W104" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="X104" s="105" t="s">
+      <c r="X104" s="108" t="s">
         <v>54</v>
       </c>
-      <c r="Y104" s="106"/>
-      <c r="Z104" s="106"/>
-      <c r="AA104" s="107"/>
-      <c r="AB104" s="108" t="s">
+      <c r="Y104" s="109"/>
+      <c r="Z104" s="109"/>
+      <c r="AA104" s="110"/>
+      <c r="AB104" s="111" t="s">
         <v>93</v>
       </c>
-      <c r="AC104" s="110" t="s">
+      <c r="AC104" s="113" t="s">
         <v>56</v>
       </c>
-      <c r="AD104" s="111"/>
-      <c r="AE104" s="111"/>
-      <c r="AF104" s="112"/>
-      <c r="AG104" s="113" t="s">
+      <c r="AD104" s="114"/>
+      <c r="AE104" s="114"/>
+      <c r="AF104" s="115"/>
+      <c r="AG104" s="116" t="s">
         <v>94</v>
       </c>
-      <c r="AH104" s="113"/>
-      <c r="AI104" s="113"/>
-      <c r="AJ104" s="113"/>
-      <c r="AK104" s="103" t="s">
+      <c r="AH104" s="116"/>
+      <c r="AI104" s="116"/>
+      <c r="AJ104" s="116"/>
+      <c r="AK104" s="102" t="s">
         <v>58</v>
       </c>
-      <c r="AL104" s="103" t="s">
+      <c r="AL104" s="102" t="s">
         <v>59</v>
       </c>
       <c r="AM104" s="64"/>
     </row>
     <row r="105" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A105" s="104"/>
+      <c r="A105" s="103"/>
       <c r="B105" s="63" t="s">
         <v>13</v>
       </c>
@@ -19038,7 +19134,7 @@
       <c r="E105" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="F105" s="109"/>
+      <c r="F105" s="112"/>
       <c r="G105" s="65" t="s">
         <v>33</v>
       </c>
@@ -19063,9 +19159,9 @@
       <c r="N105" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="O105" s="104"/>
-      <c r="P105" s="104"/>
-      <c r="W105" s="104"/>
+      <c r="O105" s="103"/>
+      <c r="P105" s="103"/>
+      <c r="W105" s="103"/>
       <c r="X105" s="63" t="s">
         <v>13</v>
       </c>
@@ -19078,7 +19174,7 @@
       <c r="AA105" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="AB105" s="109"/>
+      <c r="AB105" s="112"/>
       <c r="AC105" s="65" t="s">
         <v>33</v>
       </c>
@@ -19103,8 +19199,8 @@
       <c r="AJ105" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="AK105" s="104"/>
-      <c r="AL105" s="104"/>
+      <c r="AK105" s="103"/>
+      <c r="AL105" s="103"/>
     </row>
     <row r="106" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A106" s="66">
@@ -20054,21 +20150,21 @@
       <c r="A114" t="s">
         <v>98</v>
       </c>
-      <c r="K114" s="114" t="s">
+      <c r="K114" s="104" t="s">
         <v>99</v>
       </c>
-      <c r="L114" s="114"/>
-      <c r="M114" s="114"/>
-      <c r="N114" s="114"/>
+      <c r="L114" s="104"/>
+      <c r="M114" s="104"/>
+      <c r="N114" s="104"/>
       <c r="W114" t="s">
         <v>98</v>
       </c>
-      <c r="AG114" s="114" t="s">
+      <c r="AG114" s="104" t="s">
         <v>99</v>
       </c>
-      <c r="AH114" s="114"/>
-      <c r="AI114" s="114"/>
-      <c r="AJ114" s="114"/>
+      <c r="AH114" s="104"/>
+      <c r="AI114" s="104"/>
+      <c r="AJ114" s="104"/>
     </row>
     <row r="115" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
@@ -20088,45 +20184,53 @@
     </row>
   </sheetData>
   <mergeCells count="110">
-    <mergeCell ref="AK104:AK105"/>
-    <mergeCell ref="AL104:AL105"/>
-    <mergeCell ref="AG114:AJ114"/>
-    <mergeCell ref="AL81:AL82"/>
-    <mergeCell ref="AG91:AJ91"/>
-    <mergeCell ref="AD101:AD102"/>
-    <mergeCell ref="AJ101:AJ102"/>
-    <mergeCell ref="AN101:AN103"/>
-    <mergeCell ref="W104:W105"/>
-    <mergeCell ref="X104:AA104"/>
-    <mergeCell ref="AB104:AB105"/>
-    <mergeCell ref="AC104:AF104"/>
-    <mergeCell ref="AG104:AJ104"/>
-    <mergeCell ref="W81:W82"/>
-    <mergeCell ref="X81:AA81"/>
-    <mergeCell ref="AB81:AB82"/>
-    <mergeCell ref="AC81:AF81"/>
-    <mergeCell ref="AG81:AJ81"/>
-    <mergeCell ref="AK81:AK82"/>
-    <mergeCell ref="AL58:AL59"/>
-    <mergeCell ref="AG68:AJ68"/>
-    <mergeCell ref="AD78:AD79"/>
-    <mergeCell ref="AJ78:AJ79"/>
-    <mergeCell ref="AN78:AN80"/>
-    <mergeCell ref="AL34:AL35"/>
-    <mergeCell ref="AG44:AJ44"/>
-    <mergeCell ref="AD55:AD56"/>
-    <mergeCell ref="AJ55:AJ56"/>
-    <mergeCell ref="AN55:AN57"/>
-    <mergeCell ref="AK34:AK35"/>
-    <mergeCell ref="AB58:AB59"/>
-    <mergeCell ref="AC58:AF58"/>
-    <mergeCell ref="AG58:AJ58"/>
-    <mergeCell ref="W34:W35"/>
-    <mergeCell ref="X34:AA34"/>
-    <mergeCell ref="AB34:AB35"/>
-    <mergeCell ref="AC34:AF34"/>
-    <mergeCell ref="AG34:AJ34"/>
-    <mergeCell ref="AK58:AK59"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="R7:R9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="K10:N10"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="G34:J34"/>
+    <mergeCell ref="K34:N34"/>
+    <mergeCell ref="O34:O35"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="N31:N32"/>
+    <mergeCell ref="R31:R33"/>
+    <mergeCell ref="P34:P35"/>
+    <mergeCell ref="H78:H79"/>
+    <mergeCell ref="N78:N79"/>
+    <mergeCell ref="R78:R80"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="B81:E81"/>
+    <mergeCell ref="F81:F82"/>
+    <mergeCell ref="G81:J81"/>
+    <mergeCell ref="K81:N81"/>
+    <mergeCell ref="K44:N44"/>
+    <mergeCell ref="H55:H56"/>
+    <mergeCell ref="N55:N56"/>
+    <mergeCell ref="R55:R57"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="B58:E58"/>
+    <mergeCell ref="F58:F59"/>
+    <mergeCell ref="G58:J58"/>
+    <mergeCell ref="K58:N58"/>
+    <mergeCell ref="O58:O59"/>
+    <mergeCell ref="A104:A105"/>
+    <mergeCell ref="B104:E104"/>
+    <mergeCell ref="F104:F105"/>
+    <mergeCell ref="G104:J104"/>
+    <mergeCell ref="K104:N104"/>
+    <mergeCell ref="O104:O105"/>
+    <mergeCell ref="O81:O82"/>
+    <mergeCell ref="P81:P82"/>
+    <mergeCell ref="K91:N91"/>
+    <mergeCell ref="H101:H102"/>
+    <mergeCell ref="N101:N102"/>
     <mergeCell ref="AK10:AK11"/>
     <mergeCell ref="AL10:AL11"/>
     <mergeCell ref="AG20:AJ20"/>
@@ -20151,53 +20255,45 @@
     <mergeCell ref="K20:N20"/>
     <mergeCell ref="W58:W59"/>
     <mergeCell ref="X58:AA58"/>
-    <mergeCell ref="A104:A105"/>
-    <mergeCell ref="B104:E104"/>
-    <mergeCell ref="F104:F105"/>
-    <mergeCell ref="G104:J104"/>
-    <mergeCell ref="K104:N104"/>
-    <mergeCell ref="O104:O105"/>
-    <mergeCell ref="O81:O82"/>
-    <mergeCell ref="P81:P82"/>
-    <mergeCell ref="K91:N91"/>
-    <mergeCell ref="H101:H102"/>
-    <mergeCell ref="N101:N102"/>
-    <mergeCell ref="H78:H79"/>
-    <mergeCell ref="N78:N79"/>
-    <mergeCell ref="R78:R80"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="B81:E81"/>
-    <mergeCell ref="F81:F82"/>
-    <mergeCell ref="G81:J81"/>
-    <mergeCell ref="K81:N81"/>
-    <mergeCell ref="K44:N44"/>
-    <mergeCell ref="H55:H56"/>
-    <mergeCell ref="N55:N56"/>
-    <mergeCell ref="R55:R57"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="B58:E58"/>
-    <mergeCell ref="F58:F59"/>
-    <mergeCell ref="G58:J58"/>
-    <mergeCell ref="K58:N58"/>
-    <mergeCell ref="O58:O59"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="R7:R9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="K10:N10"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="G34:J34"/>
-    <mergeCell ref="K34:N34"/>
-    <mergeCell ref="O34:O35"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="N31:N32"/>
-    <mergeCell ref="R31:R33"/>
-    <mergeCell ref="P34:P35"/>
+    <mergeCell ref="AB58:AB59"/>
+    <mergeCell ref="AC58:AF58"/>
+    <mergeCell ref="AG58:AJ58"/>
+    <mergeCell ref="W34:W35"/>
+    <mergeCell ref="X34:AA34"/>
+    <mergeCell ref="AB34:AB35"/>
+    <mergeCell ref="AC34:AF34"/>
+    <mergeCell ref="AG34:AJ34"/>
+    <mergeCell ref="AK58:AK59"/>
+    <mergeCell ref="AL58:AL59"/>
+    <mergeCell ref="AG68:AJ68"/>
+    <mergeCell ref="AD78:AD79"/>
+    <mergeCell ref="AJ78:AJ79"/>
+    <mergeCell ref="AN78:AN80"/>
+    <mergeCell ref="AL34:AL35"/>
+    <mergeCell ref="AG44:AJ44"/>
+    <mergeCell ref="AD55:AD56"/>
+    <mergeCell ref="AJ55:AJ56"/>
+    <mergeCell ref="AN55:AN57"/>
+    <mergeCell ref="AK34:AK35"/>
+    <mergeCell ref="AK104:AK105"/>
+    <mergeCell ref="AL104:AL105"/>
+    <mergeCell ref="AG114:AJ114"/>
+    <mergeCell ref="AL81:AL82"/>
+    <mergeCell ref="AG91:AJ91"/>
+    <mergeCell ref="AD101:AD102"/>
+    <mergeCell ref="AJ101:AJ102"/>
+    <mergeCell ref="AN101:AN103"/>
+    <mergeCell ref="W104:W105"/>
+    <mergeCell ref="X104:AA104"/>
+    <mergeCell ref="AB104:AB105"/>
+    <mergeCell ref="AC104:AF104"/>
+    <mergeCell ref="AG104:AJ104"/>
+    <mergeCell ref="W81:W82"/>
+    <mergeCell ref="X81:AA81"/>
+    <mergeCell ref="AB81:AB82"/>
+    <mergeCell ref="AC81:AF81"/>
+    <mergeCell ref="AG81:AJ81"/>
+    <mergeCell ref="AK81:AK82"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20205,25 +20301,51 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3FC5E8D-5600-4792-A0B9-9888F6CE3499}">
-  <dimension ref="A1:T32"/>
+  <dimension ref="A1:X35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="18" max="18" width="48.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="84.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="43" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W1" s="118" t="s">
+        <v>144</v>
+      </c>
+      <c r="X1" s="118" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="W2" s="117" t="s">
+        <v>146</v>
+      </c>
+      <c r="X2" s="117" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="44" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W3" s="117" t="s">
+        <v>148</v>
+      </c>
+      <c r="X3" s="117" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -20236,8 +20358,14 @@
       <c r="D4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W4" s="117" t="s">
+        <v>150</v>
+      </c>
+      <c r="X4" s="117" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>83</v>
       </c>
@@ -20249,8 +20377,14 @@
       </c>
       <c r="J5" s="45"/>
       <c r="K5" s="45"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W5" s="117" t="s">
+        <v>151</v>
+      </c>
+      <c r="X5" s="117" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>85</v>
       </c>
@@ -20268,8 +20402,14 @@
       <c r="Q6" s="45" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W6" s="117" t="s">
+        <v>153</v>
+      </c>
+      <c r="X6" s="117" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>140</v>
       </c>
@@ -20281,8 +20421,14 @@
       <c r="K7" s="45"/>
       <c r="N7" s="52"/>
       <c r="Q7" s="45"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W7" s="117" t="s">
+        <v>155</v>
+      </c>
+      <c r="X7" s="117" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B8" s="45" t="s">
         <v>86</v>
       </c>
@@ -20294,7 +20440,7 @@
       </c>
       <c r="E8" s="45"/>
       <c r="F8" s="45"/>
-      <c r="I8" s="100" t="s">
+      <c r="I8" s="105" t="s">
         <v>59</v>
       </c>
       <c r="J8" s="50"/>
@@ -20306,7 +20452,7 @@
         <v>88</v>
       </c>
       <c r="N8" s="52"/>
-      <c r="Q8" s="102" t="s">
+      <c r="Q8" s="107" t="s">
         <v>59</v>
       </c>
       <c r="R8" s="51">
@@ -20315,8 +20461,14 @@
       <c r="S8" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W8" s="117" t="s">
+        <v>157</v>
+      </c>
+      <c r="X8" s="117" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>90</v>
       </c>
@@ -20326,7 +20478,7 @@
       <c r="D9" s="54"/>
       <c r="E9" s="54"/>
       <c r="F9" s="54"/>
-      <c r="I9" s="101"/>
+      <c r="I9" s="106"/>
       <c r="J9" s="55"/>
       <c r="K9" s="55"/>
       <c r="L9" s="56">
@@ -20336,15 +20488,21 @@
         <v>89</v>
       </c>
       <c r="N9" s="58"/>
-      <c r="Q9" s="102"/>
+      <c r="Q9" s="107"/>
       <c r="R9" s="51">
         <v>1</v>
       </c>
       <c r="S9" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W9" s="117" t="s">
+        <v>159</v>
+      </c>
+      <c r="X9" s="117" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C10" s="54"/>
       <c r="D10" s="54"/>
       <c r="E10" s="54"/>
@@ -20365,45 +20523,57 @@
         <v>52</v>
       </c>
       <c r="S10" s="62"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="103" t="s">
+      <c r="W10" s="117" t="s">
+        <v>161</v>
+      </c>
+      <c r="X10" s="117" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A11" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="105" t="s">
+      <c r="B11" s="108" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="106"/>
-      <c r="D11" s="106"/>
-      <c r="E11" s="106"/>
-      <c r="F11" s="107"/>
-      <c r="G11" s="108" t="s">
+      <c r="C11" s="109"/>
+      <c r="D11" s="109"/>
+      <c r="E11" s="109"/>
+      <c r="F11" s="110"/>
+      <c r="G11" s="111" t="s">
         <v>93</v>
       </c>
-      <c r="H11" s="110" t="s">
+      <c r="H11" s="113" t="s">
         <v>56</v>
       </c>
-      <c r="I11" s="111"/>
-      <c r="J11" s="111"/>
-      <c r="K11" s="111"/>
-      <c r="L11" s="112"/>
-      <c r="M11" s="113" t="s">
+      <c r="I11" s="114"/>
+      <c r="J11" s="114"/>
+      <c r="K11" s="114"/>
+      <c r="L11" s="115"/>
+      <c r="M11" s="116" t="s">
         <v>94</v>
       </c>
-      <c r="N11" s="113"/>
-      <c r="O11" s="113"/>
-      <c r="P11" s="113"/>
-      <c r="Q11" s="113"/>
-      <c r="R11" s="103" t="s">
+      <c r="N11" s="116"/>
+      <c r="O11" s="116"/>
+      <c r="P11" s="116"/>
+      <c r="Q11" s="116"/>
+      <c r="R11" s="102" t="s">
         <v>58</v>
       </c>
-      <c r="S11" s="103" t="s">
+      <c r="S11" s="102" t="s">
         <v>59</v>
       </c>
       <c r="T11" s="64"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="104"/>
+      <c r="W11" s="117" t="s">
+        <v>163</v>
+      </c>
+      <c r="X11" s="117" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12" s="103"/>
       <c r="B12" s="63" t="s">
         <v>13</v>
       </c>
@@ -20419,7 +20589,7 @@
       <c r="F12" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="G12" s="109"/>
+      <c r="G12" s="112"/>
       <c r="H12" s="65" t="s">
         <v>33</v>
       </c>
@@ -20450,10 +20620,16 @@
       <c r="Q12" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="R12" s="104"/>
-      <c r="S12" s="104"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R12" s="103"/>
+      <c r="S12" s="103"/>
+      <c r="W12" s="117" t="s">
+        <v>165</v>
+      </c>
+      <c r="X12" s="117" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="68" t="s">
         <v>123</v>
       </c>
@@ -20523,8 +20699,14 @@
         <f>IF(R13&gt;$C$8,1,0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W13" s="117" t="s">
+        <v>167</v>
+      </c>
+      <c r="X13" s="117" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="68" t="s">
         <v>124</v>
       </c>
@@ -20579,7 +20761,7 @@
         <v>-10</v>
       </c>
       <c r="P14" s="70">
-        <f t="shared" ref="P14:P28" si="2">K14+(E14*G14)</f>
+        <f>K14+(E14*G14)</f>
         <v>-5</v>
       </c>
       <c r="Q14" s="70">
@@ -20587,15 +20769,21 @@
         <v>-5</v>
       </c>
       <c r="R14" s="66">
-        <f t="shared" ref="R14:R28" si="3">$Q$28+(B14*$M$28)+(C14*$N$28)+(D14*$O$28)+(E14*$P$28)</f>
+        <f>$Q$28+(B14*$M$28)+(C14*$N$28)+(D14*$O$28)+(E14*$P$28)</f>
         <v>-0.45000000000000018</v>
       </c>
       <c r="S14" s="67">
-        <f t="shared" ref="S14:S28" si="4">IF(R14&gt;$C$8,1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+        <f>IF(R14&gt;$C$8,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="W14" s="117" t="s">
+        <v>169</v>
+      </c>
+      <c r="X14" s="117" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="68" t="s">
         <v>125</v>
       </c>
@@ -20618,23 +20806,23 @@
         <v>0</v>
       </c>
       <c r="H15" s="73">
-        <f t="shared" ref="H15:J20" si="5">M14</f>
+        <f t="shared" ref="H15:J20" si="2">M14</f>
         <v>-0.8</v>
       </c>
       <c r="I15" s="73">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>-11</v>
       </c>
       <c r="J15" s="73">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>-10</v>
       </c>
       <c r="K15" s="73">
-        <f t="shared" ref="K15:K28" si="6">P14</f>
+        <f t="shared" ref="K15:K28" si="3">P14</f>
         <v>-5</v>
       </c>
       <c r="L15" s="73">
-        <f t="shared" ref="L15:L19" si="7">Q14</f>
+        <f t="shared" ref="L15:L19" si="4">Q14</f>
         <v>-5</v>
       </c>
       <c r="M15" s="70">
@@ -20646,27 +20834,27 @@
         <v>-11</v>
       </c>
       <c r="O15" s="70">
-        <f t="shared" ref="O15:O20" si="8">J15+(D15*G15)</f>
+        <f>J15+(D15*G15)</f>
         <v>-10</v>
       </c>
       <c r="P15" s="70">
-        <f t="shared" si="2"/>
+        <f>K15+(E15*G15)</f>
         <v>-5</v>
       </c>
       <c r="Q15" s="70">
-        <f t="shared" ref="Q15:Q20" si="9">L15+(F15*G15)</f>
+        <f>L15+(F15*G15)</f>
         <v>-5</v>
       </c>
       <c r="R15" s="66">
-        <f t="shared" si="3"/>
+        <f>$Q$28+(B15*$M$28)+(C15*$N$28)+(D15*$O$28)+(E15*$P$28)</f>
         <v>-1.4500000000000002</v>
       </c>
       <c r="S15" s="67">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+        <f>IF(R15&gt;$C$8,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="68" t="s">
         <v>126</v>
       </c>
@@ -20689,23 +20877,23 @@
         <v>0</v>
       </c>
       <c r="H16" s="75">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>-0.8</v>
       </c>
       <c r="I16" s="75">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>-11</v>
       </c>
       <c r="J16" s="75">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>-10</v>
       </c>
       <c r="K16" s="75">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>-5</v>
       </c>
       <c r="L16" s="75">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>-5</v>
       </c>
       <c r="M16" s="70">
@@ -20717,23 +20905,23 @@
         <v>-11</v>
       </c>
       <c r="O16" s="70">
-        <f t="shared" si="8"/>
+        <f>J16+(D16*G16)</f>
         <v>-10</v>
       </c>
       <c r="P16" s="70">
-        <f t="shared" si="2"/>
+        <f>K16+(E16*G16)</f>
         <v>-5</v>
       </c>
       <c r="Q16" s="70">
-        <f t="shared" si="9"/>
+        <f>L16+(F16*G16)</f>
         <v>-5</v>
       </c>
       <c r="R16" s="66">
-        <f t="shared" si="3"/>
+        <f>$Q$28+(B16*$M$28)+(C16*$N$28)+(D16*$O$28)+(E16*$P$28)</f>
         <v>-0.95000000000000018</v>
       </c>
       <c r="S16" s="67">
-        <f t="shared" si="4"/>
+        <f>IF(R16&gt;$C$8,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -20760,23 +20948,23 @@
         <v>0</v>
       </c>
       <c r="H17" s="77">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>-0.8</v>
       </c>
       <c r="I17" s="77">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>-11</v>
       </c>
       <c r="J17" s="77">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>-10</v>
       </c>
       <c r="K17" s="77">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>-5</v>
       </c>
       <c r="L17" s="77">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>-5</v>
       </c>
       <c r="M17" s="70">
@@ -20788,23 +20976,23 @@
         <v>-11</v>
       </c>
       <c r="O17" s="70">
-        <f t="shared" si="8"/>
+        <f>J17+(D17*G17)</f>
         <v>-10</v>
       </c>
       <c r="P17" s="70">
-        <f t="shared" si="2"/>
+        <f>K17+(E17*G17)</f>
         <v>-5</v>
       </c>
       <c r="Q17" s="70">
-        <f t="shared" si="9"/>
+        <f>L17+(F17*G17)</f>
         <v>-5</v>
       </c>
       <c r="R17" s="66">
-        <f t="shared" si="3"/>
+        <f>$Q$28+(B17*$M$28)+(C17*$N$28)+(D17*$O$28)+(E17*$P$28)</f>
         <v>-2.95</v>
       </c>
       <c r="S17" s="67">
-        <f t="shared" si="4"/>
+        <f>IF(R17&gt;$C$8,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -20831,23 +21019,23 @@
         <v>0</v>
       </c>
       <c r="H18" s="79">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>-0.8</v>
       </c>
       <c r="I18" s="79">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>-11</v>
       </c>
       <c r="J18" s="79">
         <f>O17</f>
         <v>-10</v>
       </c>
-      <c r="K18" s="115">
-        <f t="shared" si="6"/>
+      <c r="K18" s="90">
+        <f t="shared" si="3"/>
         <v>-5</v>
       </c>
       <c r="L18" s="79">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>-5</v>
       </c>
       <c r="M18" s="70">
@@ -20859,23 +21047,23 @@
         <v>-11</v>
       </c>
       <c r="O18" s="70">
-        <f t="shared" si="8"/>
+        <f>J18+(D18*G18)</f>
         <v>-10</v>
       </c>
       <c r="P18" s="70">
-        <f t="shared" si="2"/>
+        <f>K18+(E18*G18)</f>
         <v>-5</v>
       </c>
       <c r="Q18" s="70">
-        <f t="shared" si="9"/>
+        <f>L18+(F18*G18)</f>
         <v>-5</v>
       </c>
       <c r="R18" s="66">
-        <f t="shared" si="3"/>
+        <f>$Q$28+(B18*$M$28)+(C18*$N$28)+(D18*$O$28)+(E18*$P$28)</f>
         <v>-3.2</v>
       </c>
       <c r="S18" s="67">
-        <f t="shared" si="4"/>
+        <f>IF(R18&gt;$C$8,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -20902,23 +21090,23 @@
         <v>0</v>
       </c>
       <c r="H19" s="81">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>-0.8</v>
       </c>
       <c r="I19" s="81">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>-11</v>
       </c>
       <c r="J19" s="81">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>-10</v>
       </c>
       <c r="K19" s="81">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>-5</v>
       </c>
       <c r="L19" s="81">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>-5</v>
       </c>
       <c r="M19" s="70">
@@ -20930,23 +21118,23 @@
         <v>-11</v>
       </c>
       <c r="O19" s="70">
-        <f t="shared" si="8"/>
+        <f>J19+(D19*G19)</f>
         <v>-10</v>
       </c>
       <c r="P19" s="70">
-        <f t="shared" si="2"/>
+        <f>K19+(E19*G19)</f>
         <v>-5</v>
       </c>
       <c r="Q19" s="70">
-        <f t="shared" si="9"/>
+        <f>L19+(F19*G19)</f>
         <v>-5</v>
       </c>
       <c r="R19" s="66">
-        <f t="shared" si="3"/>
+        <f>$Q$28+(B19*$M$28)+(C19*$N$28)+(D19*$O$28)+(E19*$P$28)</f>
         <v>-3.45</v>
       </c>
       <c r="S19" s="67">
-        <f t="shared" si="4"/>
+        <f>IF(R19&gt;$C$8,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -20973,19 +21161,19 @@
         <v>0</v>
       </c>
       <c r="H20" s="83">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>-0.8</v>
       </c>
       <c r="I20" s="83">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>-11</v>
       </c>
       <c r="J20" s="83">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>-10</v>
       </c>
-      <c r="K20" s="116">
-        <f t="shared" si="6"/>
+      <c r="K20" s="91">
+        <f t="shared" si="3"/>
         <v>-5</v>
       </c>
       <c r="L20" s="83">
@@ -21001,23 +21189,23 @@
         <v>-11</v>
       </c>
       <c r="O20" s="86">
-        <f t="shared" si="8"/>
+        <f>J20+(D20*G20)</f>
         <v>-10</v>
       </c>
       <c r="P20" s="87">
-        <f t="shared" si="2"/>
+        <f>K20+(E20*G20)</f>
         <v>-5</v>
       </c>
       <c r="Q20" s="86">
-        <f t="shared" si="9"/>
+        <f>L20+(F20*G20)</f>
         <v>-5</v>
       </c>
       <c r="R20" s="66">
-        <f t="shared" si="3"/>
+        <f>$Q$28+(B20*$M$28)+(C20*$N$28)+(D20*$O$28)+(E20*$P$28)</f>
         <v>-3.7</v>
       </c>
       <c r="S20" s="67">
-        <f t="shared" si="4"/>
+        <f>IF(R20&gt;$C$8,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -21044,51 +21232,51 @@
         <v>1</v>
       </c>
       <c r="H21" s="83">
-        <f t="shared" ref="H21:H28" si="10">M20</f>
+        <f t="shared" ref="H21:H28" si="5">M20</f>
         <v>-0.8</v>
       </c>
       <c r="I21" s="83">
-        <f t="shared" ref="I21:I28" si="11">N20</f>
+        <f t="shared" ref="I21:I28" si="6">N20</f>
         <v>-11</v>
       </c>
       <c r="J21" s="83">
-        <f t="shared" ref="J21:J28" si="12">O20</f>
+        <f t="shared" ref="J21:J28" si="7">O20</f>
         <v>-10</v>
       </c>
-      <c r="K21" s="116">
-        <f t="shared" si="6"/>
+      <c r="K21" s="91">
+        <f t="shared" si="3"/>
         <v>-5</v>
       </c>
       <c r="L21" s="83">
-        <f t="shared" ref="L21:L28" si="13">Q20</f>
+        <f t="shared" ref="L21:L28" si="8">Q20</f>
         <v>-5</v>
       </c>
       <c r="M21" s="86">
-        <f t="shared" ref="M21:M28" si="14">H21+(B21*G21)</f>
+        <f t="shared" ref="M21:M28" si="9">H21+(B21*G21)</f>
         <v>0.19999999999999996</v>
       </c>
       <c r="N21" s="86">
-        <f t="shared" ref="N21:N28" si="15">I21+(C21*G21)</f>
+        <f t="shared" ref="N21:N28" si="10">I21+(C21*G21)</f>
         <v>-10.5</v>
       </c>
       <c r="O21" s="86">
-        <f t="shared" ref="O21:O28" si="16">J21+(D21*G21)</f>
+        <f>J21+(D21*G21)</f>
         <v>-9.25</v>
       </c>
       <c r="P21" s="87">
-        <f t="shared" si="2"/>
+        <f>K21+(E21*G21)</f>
         <v>-4.25</v>
       </c>
       <c r="Q21" s="86">
-        <f t="shared" ref="Q21:Q28" si="17">L21+(F21*G21)</f>
+        <f>L21+(F21*G21)</f>
         <v>-4</v>
       </c>
       <c r="R21" s="66">
-        <f t="shared" si="3"/>
+        <f>$Q$28+(B21*$M$28)+(C21*$N$28)+(D21*$O$28)+(E21*$P$28)</f>
         <v>4.6999999999999993</v>
       </c>
       <c r="S21" s="67">
-        <f t="shared" si="4"/>
+        <f>IF(R21&gt;$C$8,1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -21115,51 +21303,51 @@
         <v>1</v>
       </c>
       <c r="H22" s="83">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>0.19999999999999996</v>
       </c>
       <c r="I22" s="83">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
         <v>-10.5</v>
       </c>
       <c r="J22" s="83">
         <f>O21</f>
         <v>-9.25</v>
       </c>
-      <c r="K22" s="116">
-        <f t="shared" si="6"/>
+      <c r="K22" s="91">
+        <f t="shared" si="3"/>
         <v>-4.25</v>
       </c>
       <c r="L22" s="83">
-        <f t="shared" si="13"/>
+        <f t="shared" si="8"/>
         <v>-4</v>
       </c>
       <c r="M22" s="86">
-        <f t="shared" si="14"/>
+        <f t="shared" si="9"/>
         <v>1.2</v>
       </c>
       <c r="N22" s="86">
-        <f t="shared" si="15"/>
+        <f t="shared" si="10"/>
         <v>-10</v>
       </c>
       <c r="O22" s="86">
-        <f t="shared" si="16"/>
+        <f>J22+(D22*G22)</f>
         <v>-8.5</v>
       </c>
       <c r="P22" s="87">
-        <f t="shared" si="2"/>
+        <f>K22+(E22*G22)</f>
         <v>-4</v>
       </c>
       <c r="Q22" s="86">
-        <f t="shared" si="17"/>
+        <f>L22+(F22*G22)</f>
         <v>-3</v>
       </c>
       <c r="R22" s="66">
-        <f t="shared" si="3"/>
+        <f>$Q$28+(B22*$M$28)+(C22*$N$28)+(D22*$O$28)+(E22*$P$28)</f>
         <v>5.1999999999999993</v>
       </c>
       <c r="S22" s="67">
-        <f t="shared" si="4"/>
+        <f>IF(R22&gt;$C$8,1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -21186,51 +21374,51 @@
         <v>1</v>
       </c>
       <c r="H23" s="83">
+        <f t="shared" si="5"/>
+        <v>1.2</v>
+      </c>
+      <c r="I23" s="83">
+        <f t="shared" si="6"/>
+        <v>-10</v>
+      </c>
+      <c r="J23" s="83">
+        <f t="shared" si="7"/>
+        <v>-8.5</v>
+      </c>
+      <c r="K23" s="91">
+        <f t="shared" si="3"/>
+        <v>-4</v>
+      </c>
+      <c r="L23" s="83">
+        <f t="shared" si="8"/>
+        <v>-3</v>
+      </c>
+      <c r="M23" s="86">
+        <f t="shared" si="9"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="N23" s="86">
         <f t="shared" si="10"/>
-        <v>1.2</v>
-      </c>
-      <c r="I23" s="83">
-        <f t="shared" si="11"/>
-        <v>-10</v>
-      </c>
-      <c r="J23" s="83">
-        <f t="shared" si="12"/>
-        <v>-8.5</v>
-      </c>
-      <c r="K23" s="116">
-        <f t="shared" si="6"/>
-        <v>-4</v>
-      </c>
-      <c r="L23" s="83">
-        <f t="shared" si="13"/>
-        <v>-3</v>
-      </c>
-      <c r="M23" s="86">
-        <f t="shared" si="14"/>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="N23" s="86">
-        <f t="shared" si="15"/>
         <v>-9.5</v>
       </c>
       <c r="O23" s="86">
-        <f t="shared" si="16"/>
+        <f>J23+(D23*G23)</f>
         <v>-7.5</v>
       </c>
       <c r="P23" s="87">
-        <f t="shared" si="2"/>
+        <f>K23+(E23*G23)</f>
         <v>-3.5</v>
       </c>
       <c r="Q23" s="86">
-        <f t="shared" si="17"/>
+        <f>L23+(F23*G23)</f>
         <v>-2</v>
       </c>
       <c r="R23" s="66">
-        <f t="shared" si="3"/>
+        <f>$Q$28+(B23*$M$28)+(C23*$N$28)+(D23*$O$28)+(E23*$P$28)</f>
         <v>4.1999999999999993</v>
       </c>
       <c r="S23" s="67">
-        <f t="shared" si="4"/>
+        <f>IF(R23&gt;$C$8,1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -21257,51 +21445,51 @@
         <v>1</v>
       </c>
       <c r="H24" s="83">
+        <f t="shared" si="5"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I24" s="83">
+        <f t="shared" si="6"/>
+        <v>-9.5</v>
+      </c>
+      <c r="J24" s="83">
+        <f t="shared" si="7"/>
+        <v>-7.5</v>
+      </c>
+      <c r="K24" s="91">
+        <f t="shared" si="3"/>
+        <v>-3.5</v>
+      </c>
+      <c r="L24" s="83">
+        <f t="shared" si="8"/>
+        <v>-2</v>
+      </c>
+      <c r="M24" s="86">
+        <f t="shared" si="9"/>
+        <v>3.2</v>
+      </c>
+      <c r="N24" s="86">
         <f t="shared" si="10"/>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="I24" s="83">
-        <f t="shared" si="11"/>
-        <v>-9.5</v>
-      </c>
-      <c r="J24" s="83">
-        <f t="shared" si="12"/>
-        <v>-7.5</v>
-      </c>
-      <c r="K24" s="116">
-        <f t="shared" si="6"/>
-        <v>-3.5</v>
-      </c>
-      <c r="L24" s="83">
-        <f t="shared" si="13"/>
-        <v>-2</v>
-      </c>
-      <c r="M24" s="86">
-        <f t="shared" si="14"/>
-        <v>3.2</v>
-      </c>
-      <c r="N24" s="86">
-        <f t="shared" si="15"/>
         <v>-9</v>
       </c>
       <c r="O24" s="86">
-        <f t="shared" si="16"/>
+        <f>J24+(D24*G24)</f>
         <v>-6.5</v>
       </c>
       <c r="P24" s="87">
-        <f t="shared" si="2"/>
+        <f>K24+(E24*G24)</f>
         <v>-2.75</v>
       </c>
       <c r="Q24" s="86">
-        <f t="shared" si="17"/>
+        <f>L24+(F24*G24)</f>
         <v>-1</v>
       </c>
       <c r="R24" s="66">
-        <f t="shared" si="3"/>
+        <f>$Q$28+(B24*$M$28)+(C24*$N$28)+(D24*$O$28)+(E24*$P$28)</f>
         <v>3.9499999999999993</v>
       </c>
       <c r="S24" s="67">
-        <f t="shared" si="4"/>
+        <f>IF(R24&gt;$C$8,1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -21328,51 +21516,51 @@
         <v>1</v>
       </c>
       <c r="H25" s="83">
+        <f t="shared" si="5"/>
+        <v>3.2</v>
+      </c>
+      <c r="I25" s="83">
+        <f t="shared" si="6"/>
+        <v>-9</v>
+      </c>
+      <c r="J25" s="83">
+        <f t="shared" si="7"/>
+        <v>-6.5</v>
+      </c>
+      <c r="K25" s="91">
+        <f t="shared" si="3"/>
+        <v>-2.75</v>
+      </c>
+      <c r="L25" s="83">
+        <f t="shared" si="8"/>
+        <v>-1</v>
+      </c>
+      <c r="M25" s="86">
+        <f t="shared" si="9"/>
+        <v>4.2</v>
+      </c>
+      <c r="N25" s="86">
         <f t="shared" si="10"/>
-        <v>3.2</v>
-      </c>
-      <c r="I25" s="83">
-        <f t="shared" si="11"/>
-        <v>-9</v>
-      </c>
-      <c r="J25" s="83">
-        <f t="shared" si="12"/>
-        <v>-6.5</v>
-      </c>
-      <c r="K25" s="116">
-        <f t="shared" si="6"/>
-        <v>-2.75</v>
-      </c>
-      <c r="L25" s="83">
-        <f t="shared" si="13"/>
-        <v>-1</v>
-      </c>
-      <c r="M25" s="86">
-        <f t="shared" si="14"/>
-        <v>4.2</v>
-      </c>
-      <c r="N25" s="86">
-        <f t="shared" si="15"/>
         <v>-8</v>
       </c>
       <c r="O25" s="86">
-        <f t="shared" si="16"/>
+        <f>J25+(D25*G25)</f>
         <v>-5.75</v>
       </c>
       <c r="P25" s="87">
-        <f t="shared" si="2"/>
+        <f>K25+(E25*G25)</f>
         <v>-2.5</v>
       </c>
       <c r="Q25" s="86">
-        <f t="shared" si="17"/>
+        <f>L25+(F25*G25)</f>
         <v>0</v>
       </c>
       <c r="R25" s="66">
-        <f t="shared" si="3"/>
+        <f>$Q$28+(B25*$M$28)+(C25*$N$28)+(D25*$O$28)+(E25*$P$28)</f>
         <v>2.6999999999999993</v>
       </c>
       <c r="S25" s="67">
-        <f t="shared" si="4"/>
+        <f>IF(R25&gt;$C$8,1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -21399,51 +21587,51 @@
         <v>1</v>
       </c>
       <c r="H26" s="83">
+        <f t="shared" si="5"/>
+        <v>4.2</v>
+      </c>
+      <c r="I26" s="83">
+        <f t="shared" si="6"/>
+        <v>-8</v>
+      </c>
+      <c r="J26" s="83">
+        <f t="shared" si="7"/>
+        <v>-5.75</v>
+      </c>
+      <c r="K26" s="91">
+        <f t="shared" si="3"/>
+        <v>-2.5</v>
+      </c>
+      <c r="L26" s="83">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="M26" s="86">
+        <f t="shared" si="9"/>
+        <v>5.2</v>
+      </c>
+      <c r="N26" s="86">
         <f t="shared" si="10"/>
-        <v>4.2</v>
-      </c>
-      <c r="I26" s="83">
-        <f t="shared" si="11"/>
-        <v>-8</v>
-      </c>
-      <c r="J26" s="83">
-        <f t="shared" si="12"/>
-        <v>-5.75</v>
-      </c>
-      <c r="K26" s="116">
-        <f t="shared" si="6"/>
-        <v>-2.5</v>
-      </c>
-      <c r="L26" s="83">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="M26" s="86">
-        <f t="shared" si="14"/>
-        <v>5.2</v>
-      </c>
-      <c r="N26" s="86">
-        <f t="shared" si="15"/>
         <v>-7</v>
       </c>
       <c r="O26" s="86">
-        <f t="shared" si="16"/>
+        <f>J26+(D26*G26)</f>
         <v>-5</v>
       </c>
       <c r="P26" s="87">
-        <f t="shared" si="2"/>
+        <f>K26+(E26*G26)</f>
         <v>-2</v>
       </c>
       <c r="Q26" s="86">
-        <f t="shared" si="17"/>
+        <f>L26+(F26*G26)</f>
         <v>1</v>
       </c>
       <c r="R26" s="66">
-        <f t="shared" si="3"/>
+        <f>$Q$28+(B26*$M$28)+(C26*$N$28)+(D26*$O$28)+(E26*$P$28)</f>
         <v>2.4499999999999993</v>
       </c>
       <c r="S26" s="67">
-        <f t="shared" si="4"/>
+        <f>IF(R26&gt;$C$8,1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -21470,51 +21658,51 @@
         <v>1</v>
       </c>
       <c r="H27" s="83">
+        <f t="shared" si="5"/>
+        <v>5.2</v>
+      </c>
+      <c r="I27" s="83">
+        <f t="shared" si="6"/>
+        <v>-7</v>
+      </c>
+      <c r="J27" s="83">
+        <f t="shared" si="7"/>
+        <v>-5</v>
+      </c>
+      <c r="K27" s="91">
+        <f t="shared" si="3"/>
+        <v>-2</v>
+      </c>
+      <c r="L27" s="83">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="M27" s="86">
+        <f t="shared" si="9"/>
+        <v>6.2</v>
+      </c>
+      <c r="N27" s="86">
         <f t="shared" si="10"/>
-        <v>5.2</v>
-      </c>
-      <c r="I27" s="83">
-        <f t="shared" si="11"/>
-        <v>-7</v>
-      </c>
-      <c r="J27" s="83">
-        <f t="shared" si="12"/>
-        <v>-5</v>
-      </c>
-      <c r="K27" s="116">
-        <f t="shared" si="6"/>
-        <v>-2</v>
-      </c>
-      <c r="L27" s="83">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-      <c r="M27" s="86">
-        <f t="shared" si="14"/>
-        <v>6.2</v>
-      </c>
-      <c r="N27" s="86">
-        <f t="shared" si="15"/>
         <v>-6</v>
       </c>
       <c r="O27" s="86">
-        <f t="shared" si="16"/>
+        <f>J27+(D27*G27)</f>
         <v>-4</v>
       </c>
       <c r="P27" s="87">
-        <f t="shared" si="2"/>
+        <f>K27+(E27*G27)</f>
         <v>-1.25</v>
       </c>
       <c r="Q27" s="86">
-        <f t="shared" si="17"/>
+        <f>L27+(F27*G27)</f>
         <v>2</v>
       </c>
       <c r="R27" s="66">
-        <f t="shared" si="3"/>
+        <f>$Q$28+(B27*$M$28)+(C27*$N$28)+(D27*$O$28)+(E27*$P$28)</f>
         <v>1.4499999999999993</v>
       </c>
       <c r="S27" s="67">
-        <f t="shared" si="4"/>
+        <f>IF(R27&gt;$C$8,1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -21541,51 +21729,51 @@
         <v>1</v>
       </c>
       <c r="H28" s="83">
+        <f t="shared" si="5"/>
+        <v>6.2</v>
+      </c>
+      <c r="I28" s="83">
+        <f t="shared" si="6"/>
+        <v>-6</v>
+      </c>
+      <c r="J28" s="83">
+        <f t="shared" si="7"/>
+        <v>-4</v>
+      </c>
+      <c r="K28" s="91">
+        <f t="shared" si="3"/>
+        <v>-1.25</v>
+      </c>
+      <c r="L28" s="83">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="M28" s="88">
+        <f t="shared" si="9"/>
+        <v>7.2</v>
+      </c>
+      <c r="N28" s="88">
         <f t="shared" si="10"/>
-        <v>6.2</v>
-      </c>
-      <c r="I28" s="83">
-        <f t="shared" si="11"/>
-        <v>-6</v>
-      </c>
-      <c r="J28" s="83">
-        <f t="shared" si="12"/>
-        <v>-4</v>
-      </c>
-      <c r="K28" s="116">
-        <f t="shared" si="6"/>
-        <v>-1.25</v>
-      </c>
-      <c r="L28" s="83">
-        <f t="shared" si="13"/>
-        <v>2</v>
-      </c>
-      <c r="M28" s="88">
-        <f t="shared" si="14"/>
-        <v>7.2</v>
-      </c>
-      <c r="N28" s="88">
-        <f t="shared" si="15"/>
         <v>-5</v>
       </c>
       <c r="O28" s="88">
-        <f t="shared" si="16"/>
+        <f>J28+(D28*G28)</f>
         <v>-3</v>
       </c>
       <c r="P28" s="89">
-        <f t="shared" si="2"/>
+        <f>K28+(E28*G28)</f>
         <v>-1</v>
       </c>
       <c r="Q28" s="88">
-        <f t="shared" si="17"/>
+        <f>L28+(F28*G28)</f>
         <v>3</v>
       </c>
       <c r="R28" s="66">
-        <f t="shared" si="3"/>
+        <f>$Q$28+(B28*$M$28)+(C28*$N$28)+(D28*$O$28)+(E28*$P$28)</f>
         <v>1.9499999999999993</v>
       </c>
       <c r="S28" s="67">
-        <f t="shared" si="4"/>
+        <f>IF(R28&gt;$C$8,1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -21593,36 +21781,176 @@
       <c r="A29" t="s">
         <v>98</v>
       </c>
-      <c r="M29" s="114" t="s">
+      <c r="M29" s="104" t="s">
         <v>99</v>
       </c>
-      <c r="N29" s="114"/>
-      <c r="O29" s="114"/>
-      <c r="P29" s="114"/>
-      <c r="Q29" s="114"/>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>100</v>
-      </c>
+      <c r="N29" s="104"/>
+      <c r="O29" s="104"/>
+      <c r="P29" s="104"/>
+      <c r="Q29" s="104"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32" s="45" t="s">
-        <v>101</v>
+      <c r="A32" s="45"/>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A34" s="68" t="s">
+        <v>142</v>
+      </c>
+      <c r="B34" s="66">
+        <v>1</v>
+      </c>
+      <c r="C34" s="66">
+        <v>0.25</v>
+      </c>
+      <c r="D34" s="66">
+        <v>0.75</v>
+      </c>
+      <c r="E34" s="66">
+        <v>0.75</v>
+      </c>
+      <c r="F34" s="66">
+        <v>1</v>
+      </c>
+      <c r="G34" s="67">
+        <v>1</v>
+      </c>
+      <c r="H34" s="83">
+        <f>M28</f>
+        <v>7.2</v>
+      </c>
+      <c r="I34" s="83">
+        <f t="shared" ref="I34:L34" si="11">N28</f>
+        <v>-5</v>
+      </c>
+      <c r="J34" s="83">
+        <f t="shared" si="11"/>
+        <v>-3</v>
+      </c>
+      <c r="K34" s="83">
+        <f t="shared" si="11"/>
+        <v>-1</v>
+      </c>
+      <c r="L34" s="83">
+        <f t="shared" si="11"/>
+        <v>3</v>
+      </c>
+      <c r="M34" s="86">
+        <f t="shared" ref="M34:M35" si="12">H34+(B34*G34)</f>
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="N34" s="86">
+        <f t="shared" ref="N34:N35" si="13">I34+(C34*G34)</f>
+        <v>-4.75</v>
+      </c>
+      <c r="O34" s="86">
+        <f>J34+(D34*G34)</f>
+        <v>-2.25</v>
+      </c>
+      <c r="P34" s="87">
+        <f>K34+(E34*G34)</f>
+        <v>-0.25</v>
+      </c>
+      <c r="Q34" s="86">
+        <f>L34+(F34*G34)</f>
+        <v>4</v>
+      </c>
+      <c r="R34" s="66">
+        <f>$Q$28+(B34*$M$28)+(C34*$N$28)+(D34*$O$28)+(E34*$P$28)</f>
+        <v>5.9499999999999993</v>
+      </c>
+      <c r="S34" s="67">
+        <f>IF(R34&gt;$C$8,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A35" s="68" t="s">
+        <v>143</v>
+      </c>
+      <c r="B35" s="66">
+        <v>0.25</v>
+      </c>
+      <c r="C35" s="66">
+        <v>1</v>
+      </c>
+      <c r="D35" s="66">
+        <v>0.75</v>
+      </c>
+      <c r="E35" s="66">
+        <v>0.25</v>
+      </c>
+      <c r="F35" s="66">
+        <v>1</v>
+      </c>
+      <c r="G35" s="67">
+        <v>0</v>
+      </c>
+      <c r="H35" s="83">
+        <f>M34</f>
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="I35" s="83">
+        <f t="shared" ref="I35" si="14">N34</f>
+        <v>-4.75</v>
+      </c>
+      <c r="J35" s="83">
+        <f t="shared" ref="J35" si="15">O34</f>
+        <v>-2.25</v>
+      </c>
+      <c r="K35" s="91">
+        <f t="shared" ref="K35" si="16">P34</f>
+        <v>-0.25</v>
+      </c>
+      <c r="L35" s="83">
+        <f t="shared" ref="L35" si="17">Q34</f>
+        <v>4</v>
+      </c>
+      <c r="M35" s="88">
+        <f t="shared" si="12"/>
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="N35" s="88">
+        <f t="shared" si="13"/>
+        <v>-4.75</v>
+      </c>
+      <c r="O35" s="88">
+        <f>J35+(D35*G35)</f>
+        <v>-2.25</v>
+      </c>
+      <c r="P35" s="89">
+        <f>K35+(E35*G35)</f>
+        <v>-0.25</v>
+      </c>
+      <c r="Q35" s="88">
+        <f>L35+(F35*G35)</f>
+        <v>4</v>
+      </c>
+      <c r="R35" s="66">
+        <f>$Q$28+(B35*$M$28)+(C35*$N$28)+(D35*$O$28)+(E35*$P$28)</f>
+        <v>-2.7</v>
+      </c>
+      <c r="S35" s="67">
+        <f>IF(R35&gt;$C$8,1,0)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="R11:R12"/>
+    <mergeCell ref="S11:S12"/>
+    <mergeCell ref="M29:Q29"/>
+    <mergeCell ref="Q8:Q9"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="H11:L11"/>
     <mergeCell ref="M11:Q11"/>
-    <mergeCell ref="R11:R12"/>
-    <mergeCell ref="S11:S12"/>
-    <mergeCell ref="M29:Q29"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="Q8:Q9"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>